<commit_message>
aparapi benchmark in xls; filled abstraction part and started with hybrid cloud part
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17660" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
     <sheet name="dopencl summary" sheetId="2" r:id="rId2"/>
     <sheet name="Aparapi Matrix" sheetId="3" r:id="rId3"/>
+    <sheet name="Sharded Matrix" sheetId="4" r:id="rId4"/>
+    <sheet name="cluster ut" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Local</t>
   </si>
@@ -107,20 +109,29 @@
     <t>Aparapi small kernel small data</t>
   </si>
   <si>
-    <t>Aparapi large kernel small data</t>
-  </si>
-  <si>
     <t>Aparapi</t>
   </si>
   <si>
     <t>Original</t>
+  </si>
+  <si>
+    <t>2 Devices 1Gbit</t>
+  </si>
+  <si>
+    <t>Single Device</t>
+  </si>
+  <si>
+    <t>Aparapi &gt;100lines</t>
+  </si>
+  <si>
+    <t>Aparapi &gt;1000lines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +166,35 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF010000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF41286F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF41286F"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -173,7 +213,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="589">
+  <cellStyleXfs count="619">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -763,13 +803,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="589">
+  <cellStyles count="619">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1064,6 +1143,21 @@
     <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1358,6 +1452,21 @@
     <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1947,7 +2056,7 @@
         <v>5.4855600000000004</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J20" si="0">H12-F12-D12-B12</f>
+        <f t="shared" ref="J12:J18" si="0">H12-F12-D12-B12</f>
         <v>168.69300000000001</v>
       </c>
       <c r="N12">
@@ -1978,7 +2087,7 @@
         <v>3.9483299999999999</v>
       </c>
       <c r="W12">
-        <f t="shared" ref="W12:W20" si="1">U12-S12-Q12-O12</f>
+        <f t="shared" ref="W12:W18" si="1">U12-S12-Q12-O12</f>
         <v>146.13327000000001</v>
       </c>
     </row>
@@ -2373,7 +2482,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
-        <f t="shared" ref="C19:G19" si="2">D18/$H$18</f>
+        <f t="shared" ref="D19:F19" si="2">D18/$H$18</f>
         <v>9.323140963222476E-2</v>
       </c>
       <c r="E19" s="2"/>
@@ -2387,7 +2496,7 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2">
-        <f t="shared" ref="P19:U19" si="3">Q18/$U$18</f>
+        <f t="shared" ref="Q19:S19" si="3">Q18/$U$18</f>
         <v>4.7051349787405336E-3</v>
       </c>
       <c r="R19" s="2"/>
@@ -3070,7 +3179,7 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
-        <f t="shared" ref="C45:G45" si="6">D44/$H$44</f>
+        <f t="shared" ref="D45:F45" si="6">D44/$H$44</f>
         <v>1.402190773473257E-3</v>
       </c>
       <c r="E45" s="2"/>
@@ -4166,26 +4275,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N203"/>
+  <dimension ref="A1:P204"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
       <c r="I1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -4199,7 +4308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -4220,7 +4329,7 @@
         <v>1.0863982167950768</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -4244,7 +4353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>3000</v>
       </c>
@@ -4279,7 +4388,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>4000</v>
       </c>
@@ -4302,8 +4411,11 @@
       <c r="L6">
         <v>185</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>5000</v>
       </c>
@@ -4324,7 +4436,7 @@
         <v>1.0281690140845072</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="L7">
         <v>192</v>
@@ -4333,7 +4445,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>6000</v>
       </c>
@@ -4364,8 +4476,11 @@
       <c r="L8">
         <v>178</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>7000</v>
       </c>
@@ -4392,7 +4507,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>8000</v>
       </c>
@@ -4412,11 +4527,25 @@
         <f t="shared" si="0"/>
         <v>0.6521853607161664</v>
       </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
       <c r="L10">
         <v>214</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="P10">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="I11">
+        <f>AVERAGE(P:P)</f>
+        <v>500.69</v>
+      </c>
+      <c r="J11">
+        <f>STDEV(P:P)</f>
+        <v>15.120188524290995</v>
+      </c>
       <c r="L11">
         <v>194</v>
       </c>
@@ -4424,12 +4553,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:16">
       <c r="L12">
         <v>182</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="P12">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="L13">
         <v>198</v>
       </c>
@@ -4437,12 +4569,15 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:16">
       <c r="L14">
         <v>195</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="P14">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="L15">
         <v>215</v>
       </c>
@@ -4450,12 +4585,15 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:16">
       <c r="L16">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="12:14">
+      <c r="P16">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17" spans="12:16">
       <c r="L17">
         <v>208</v>
       </c>
@@ -4463,12 +4601,15 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="12:14">
+    <row r="18" spans="12:16">
       <c r="L18">
         <v>210</v>
       </c>
-    </row>
-    <row r="19" spans="12:14">
+      <c r="P18">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="19" spans="12:16">
       <c r="L19">
         <v>196</v>
       </c>
@@ -4476,12 +4617,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="12:14">
+    <row r="20" spans="12:16">
       <c r="L20">
         <v>202</v>
       </c>
-    </row>
-    <row r="21" spans="12:14">
+      <c r="P20">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="21" spans="12:16">
       <c r="L21">
         <v>192</v>
       </c>
@@ -4489,12 +4633,15 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="12:14">
+    <row r="22" spans="12:16">
       <c r="L22">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="12:14">
+      <c r="P22">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="23" spans="12:16">
       <c r="L23">
         <v>185</v>
       </c>
@@ -4502,12 +4649,15 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="12:14">
+    <row r="24" spans="12:16">
       <c r="L24">
         <v>208</v>
       </c>
-    </row>
-    <row r="25" spans="12:14">
+      <c r="P24">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="12:16">
       <c r="L25">
         <v>197</v>
       </c>
@@ -4515,12 +4665,15 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="12:14">
+    <row r="26" spans="12:16">
       <c r="L26">
         <v>211</v>
       </c>
-    </row>
-    <row r="27" spans="12:14">
+      <c r="P26">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="27" spans="12:16">
       <c r="L27">
         <v>199</v>
       </c>
@@ -4528,12 +4681,15 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="12:14">
+    <row r="28" spans="12:16">
       <c r="L28">
         <v>211</v>
       </c>
-    </row>
-    <row r="29" spans="12:14">
+      <c r="P28">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="12:16">
       <c r="L29">
         <v>185</v>
       </c>
@@ -4541,12 +4697,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="12:14">
+    <row r="30" spans="12:16">
       <c r="L30">
         <v>214</v>
       </c>
-    </row>
-    <row r="31" spans="12:14">
+      <c r="P30">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="31" spans="12:16">
       <c r="L31">
         <v>192</v>
       </c>
@@ -4554,12 +4713,15 @@
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="12:14">
+    <row r="32" spans="12:16">
       <c r="L32">
         <v>193</v>
       </c>
-    </row>
-    <row r="33" spans="12:14">
+      <c r="P32">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="33" spans="12:16">
       <c r="L33">
         <v>194</v>
       </c>
@@ -4567,12 +4729,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="34" spans="12:14">
+    <row r="34" spans="12:16">
       <c r="L34">
         <v>213</v>
       </c>
-    </row>
-    <row r="35" spans="12:14">
+      <c r="P34">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="35" spans="12:16">
       <c r="L35">
         <v>210</v>
       </c>
@@ -4580,12 +4745,15 @@
         <v>257</v>
       </c>
     </row>
-    <row r="36" spans="12:14">
+    <row r="36" spans="12:16">
       <c r="L36">
         <v>197</v>
       </c>
-    </row>
-    <row r="37" spans="12:14">
+      <c r="P36">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="37" spans="12:16">
       <c r="L37">
         <v>209</v>
       </c>
@@ -4593,12 +4761,15 @@
         <v>270</v>
       </c>
     </row>
-    <row r="38" spans="12:14">
+    <row r="38" spans="12:16">
       <c r="L38">
         <v>186</v>
       </c>
-    </row>
-    <row r="39" spans="12:14">
+      <c r="P38">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="39" spans="12:16">
       <c r="L39">
         <v>197</v>
       </c>
@@ -4606,12 +4777,15 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="12:14">
+    <row r="40" spans="12:16">
       <c r="L40">
         <v>194</v>
       </c>
-    </row>
-    <row r="41" spans="12:14">
+      <c r="P40">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="41" spans="12:16">
       <c r="L41">
         <v>203</v>
       </c>
@@ -4619,12 +4793,15 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="12:14">
+    <row r="42" spans="12:16">
       <c r="L42">
         <v>214</v>
       </c>
-    </row>
-    <row r="43" spans="12:14">
+      <c r="P42">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="43" spans="12:16">
       <c r="L43">
         <v>208</v>
       </c>
@@ -4632,12 +4809,15 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="12:14">
+    <row r="44" spans="12:16">
       <c r="L44">
         <v>187</v>
       </c>
-    </row>
-    <row r="45" spans="12:14">
+      <c r="P44">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="45" spans="12:16">
       <c r="L45">
         <v>210</v>
       </c>
@@ -4645,12 +4825,15 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="12:14">
+    <row r="46" spans="12:16">
       <c r="L46">
         <v>182</v>
       </c>
-    </row>
-    <row r="47" spans="12:14">
+      <c r="P46">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="47" spans="12:16">
       <c r="L47">
         <v>197</v>
       </c>
@@ -4658,12 +4841,15 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="12:14">
+    <row r="48" spans="12:16">
       <c r="L48">
         <v>193</v>
       </c>
-    </row>
-    <row r="49" spans="12:14">
+      <c r="P48">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="49" spans="12:16">
       <c r="L49">
         <v>214</v>
       </c>
@@ -4671,12 +4857,15 @@
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="12:14">
+    <row r="50" spans="12:16">
       <c r="L50">
         <v>188</v>
       </c>
-    </row>
-    <row r="51" spans="12:14">
+      <c r="P50">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="51" spans="12:16">
       <c r="L51">
         <v>224</v>
       </c>
@@ -4684,12 +4873,15 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="12:14">
+    <row r="52" spans="12:16">
       <c r="L52">
         <v>213</v>
       </c>
-    </row>
-    <row r="53" spans="12:14">
+      <c r="P52">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="53" spans="12:16">
       <c r="L53">
         <v>194</v>
       </c>
@@ -4697,12 +4889,15 @@
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="12:14">
+    <row r="54" spans="12:16">
       <c r="L54">
         <v>177</v>
       </c>
-    </row>
-    <row r="55" spans="12:14">
+      <c r="P54">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="55" spans="12:16">
       <c r="L55">
         <v>178</v>
       </c>
@@ -4710,12 +4905,15 @@
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="12:14">
+    <row r="56" spans="12:16">
       <c r="L56">
         <v>214</v>
       </c>
-    </row>
-    <row r="57" spans="12:14">
+      <c r="P56">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="57" spans="12:16">
       <c r="L57">
         <v>190</v>
       </c>
@@ -4723,12 +4921,15 @@
         <v>247</v>
       </c>
     </row>
-    <row r="58" spans="12:14">
+    <row r="58" spans="12:16">
       <c r="L58">
         <v>223</v>
       </c>
-    </row>
-    <row r="59" spans="12:14">
+      <c r="P58">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="59" spans="12:16">
       <c r="L59">
         <v>202</v>
       </c>
@@ -4736,12 +4937,15 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="12:14">
+    <row r="60" spans="12:16">
       <c r="L60">
         <v>209</v>
       </c>
-    </row>
-    <row r="61" spans="12:14">
+      <c r="P60">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="61" spans="12:16">
       <c r="L61">
         <v>187</v>
       </c>
@@ -4749,12 +4953,15 @@
         <v>277</v>
       </c>
     </row>
-    <row r="62" spans="12:14">
+    <row r="62" spans="12:16">
       <c r="L62">
         <v>220</v>
       </c>
-    </row>
-    <row r="63" spans="12:14">
+      <c r="P62">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="63" spans="12:16">
       <c r="L63">
         <v>191</v>
       </c>
@@ -4762,12 +4969,15 @@
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="12:14">
+    <row r="64" spans="12:16">
       <c r="L64">
         <v>210</v>
       </c>
-    </row>
-    <row r="65" spans="12:14">
+      <c r="P64">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="65" spans="12:16">
       <c r="L65">
         <v>179</v>
       </c>
@@ -4775,12 +4985,15 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="12:14">
+    <row r="66" spans="12:16">
       <c r="L66">
         <v>210</v>
       </c>
-    </row>
-    <row r="67" spans="12:14">
+      <c r="P66">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="67" spans="12:16">
       <c r="L67">
         <v>193</v>
       </c>
@@ -4788,12 +5001,15 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="12:14">
+    <row r="68" spans="12:16">
       <c r="L68">
         <v>182</v>
       </c>
-    </row>
-    <row r="69" spans="12:14">
+      <c r="P68">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="69" spans="12:16">
       <c r="L69">
         <v>218</v>
       </c>
@@ -4801,12 +5017,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="12:14">
+    <row r="70" spans="12:16">
       <c r="L70">
         <v>226</v>
       </c>
-    </row>
-    <row r="71" spans="12:14">
+      <c r="P70">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="71" spans="12:16">
       <c r="L71">
         <v>204</v>
       </c>
@@ -4814,12 +5033,15 @@
         <v>253</v>
       </c>
     </row>
-    <row r="72" spans="12:14">
+    <row r="72" spans="12:16">
       <c r="L72">
         <v>198</v>
       </c>
-    </row>
-    <row r="73" spans="12:14">
+      <c r="P72">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="73" spans="12:16">
       <c r="L73">
         <v>196</v>
       </c>
@@ -4827,12 +5049,15 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="12:14">
+    <row r="74" spans="12:16">
       <c r="L74">
         <v>176</v>
       </c>
-    </row>
-    <row r="75" spans="12:14">
+      <c r="P74">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="75" spans="12:16">
       <c r="L75">
         <v>194</v>
       </c>
@@ -4840,12 +5065,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="12:14">
+    <row r="76" spans="12:16">
       <c r="L76">
         <v>191</v>
       </c>
-    </row>
-    <row r="77" spans="12:14">
+      <c r="P76">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="77" spans="12:16">
       <c r="L77">
         <v>204</v>
       </c>
@@ -4853,12 +5081,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="78" spans="12:14">
+    <row r="78" spans="12:16">
       <c r="L78">
         <v>212</v>
       </c>
-    </row>
-    <row r="79" spans="12:14">
+      <c r="P78">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="79" spans="12:16">
       <c r="L79">
         <v>213</v>
       </c>
@@ -4866,12 +5097,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="80" spans="12:14">
+    <row r="80" spans="12:16">
       <c r="L80">
         <v>192</v>
       </c>
-    </row>
-    <row r="81" spans="12:14">
+      <c r="P80">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="81" spans="12:16">
       <c r="L81">
         <v>210</v>
       </c>
@@ -4879,12 +5113,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="12:14">
+    <row r="82" spans="12:16">
       <c r="L82">
         <v>212</v>
       </c>
-    </row>
-    <row r="83" spans="12:14">
+      <c r="P82">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="83" spans="12:16">
       <c r="L83">
         <v>181</v>
       </c>
@@ -4892,12 +5129,15 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="12:14">
+    <row r="84" spans="12:16">
       <c r="L84">
         <v>190</v>
       </c>
-    </row>
-    <row r="85" spans="12:14">
+      <c r="P84">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="85" spans="12:16">
       <c r="L85">
         <v>193</v>
       </c>
@@ -4905,12 +5145,15 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="12:14">
+    <row r="86" spans="12:16">
       <c r="L86">
         <v>186</v>
       </c>
-    </row>
-    <row r="87" spans="12:14">
+      <c r="P86">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="87" spans="12:16">
       <c r="L87">
         <v>195</v>
       </c>
@@ -4918,12 +5161,15 @@
         <v>232</v>
       </c>
     </row>
-    <row r="88" spans="12:14">
+    <row r="88" spans="12:16">
       <c r="L88">
         <v>214</v>
       </c>
-    </row>
-    <row r="89" spans="12:14">
+      <c r="P88">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="89" spans="12:16">
       <c r="L89">
         <v>207</v>
       </c>
@@ -4931,12 +5177,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="12:14">
+    <row r="90" spans="12:16">
       <c r="L90">
         <v>207</v>
       </c>
-    </row>
-    <row r="91" spans="12:14">
+      <c r="P90">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="91" spans="12:16">
       <c r="L91">
         <v>210</v>
       </c>
@@ -4944,12 +5193,15 @@
         <v>264</v>
       </c>
     </row>
-    <row r="92" spans="12:14">
+    <row r="92" spans="12:16">
       <c r="L92">
         <v>220</v>
       </c>
-    </row>
-    <row r="93" spans="12:14">
+      <c r="P92">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="93" spans="12:16">
       <c r="L93">
         <v>181</v>
       </c>
@@ -4957,12 +5209,15 @@
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="12:14">
+    <row r="94" spans="12:16">
       <c r="L94">
         <v>209</v>
       </c>
-    </row>
-    <row r="95" spans="12:14">
+      <c r="P94">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="95" spans="12:16">
       <c r="L95">
         <v>220</v>
       </c>
@@ -4970,12 +5225,15 @@
         <v>230</v>
       </c>
     </row>
-    <row r="96" spans="12:14">
+    <row r="96" spans="12:16">
       <c r="L96">
         <v>195</v>
       </c>
-    </row>
-    <row r="97" spans="12:14">
+      <c r="P96">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="97" spans="12:16">
       <c r="L97">
         <v>197</v>
       </c>
@@ -4983,12 +5241,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="12:14">
+    <row r="98" spans="12:16">
       <c r="L98">
         <v>209</v>
       </c>
-    </row>
-    <row r="99" spans="12:14">
+      <c r="P98">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="99" spans="12:16">
       <c r="L99">
         <v>188</v>
       </c>
@@ -4996,12 +5257,15 @@
         <v>233</v>
       </c>
     </row>
-    <row r="100" spans="12:14">
+    <row r="100" spans="12:16">
       <c r="L100">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="12:14">
+      <c r="P100">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="101" spans="12:16">
       <c r="L101">
         <v>177</v>
       </c>
@@ -5009,12 +5273,15 @@
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="12:14">
+    <row r="102" spans="12:16">
       <c r="L102">
         <v>191</v>
       </c>
-    </row>
-    <row r="103" spans="12:14">
+      <c r="P102">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="103" spans="12:16">
       <c r="L103">
         <v>209</v>
       </c>
@@ -5022,259 +5289,512 @@
         <v>218</v>
       </c>
     </row>
-    <row r="104" spans="12:14">
+    <row r="104" spans="12:16">
       <c r="L104">
         <v>216</v>
       </c>
-    </row>
-    <row r="105" spans="12:14">
+      <c r="P104">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="105" spans="12:16">
       <c r="N105">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="12:14">
+    <row r="106" spans="12:16">
+      <c r="P106">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="107" spans="12:16">
       <c r="N107">
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="12:14">
+    <row r="108" spans="12:16">
+      <c r="P108">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="109" spans="12:16">
       <c r="N109">
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="12:14">
+    <row r="110" spans="12:16">
+      <c r="P110">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="111" spans="12:16">
       <c r="N111">
         <v>253</v>
       </c>
     </row>
-    <row r="113" spans="14:14">
+    <row r="112" spans="12:16">
+      <c r="P112">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="113" spans="14:16">
       <c r="N113">
         <v>233</v>
       </c>
     </row>
-    <row r="115" spans="14:14">
+    <row r="114" spans="14:16">
+      <c r="P114">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="115" spans="14:16">
       <c r="N115">
         <v>276</v>
       </c>
     </row>
-    <row r="117" spans="14:14">
+    <row r="116" spans="14:16">
+      <c r="P116">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="117" spans="14:16">
       <c r="N117">
         <v>233</v>
       </c>
     </row>
-    <row r="119" spans="14:14">
+    <row r="118" spans="14:16">
+      <c r="P118">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="119" spans="14:16">
       <c r="N119">
         <v>248</v>
       </c>
     </row>
-    <row r="121" spans="14:14">
+    <row r="120" spans="14:16">
+      <c r="P120">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="121" spans="14:16">
       <c r="N121">
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="14:14">
+    <row r="122" spans="14:16">
+      <c r="P122">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="123" spans="14:16">
       <c r="N123">
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="14:14">
+    <row r="124" spans="14:16">
+      <c r="P124">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="125" spans="14:16">
       <c r="N125">
         <v>254</v>
       </c>
     </row>
-    <row r="127" spans="14:14">
+    <row r="126" spans="14:16">
+      <c r="P126">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="127" spans="14:16">
       <c r="N127">
         <v>233</v>
       </c>
     </row>
-    <row r="129" spans="14:14">
+    <row r="128" spans="14:16">
+      <c r="P128">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="129" spans="14:16">
       <c r="N129">
         <v>261</v>
       </c>
     </row>
-    <row r="131" spans="14:14">
+    <row r="130" spans="14:16">
+      <c r="P130">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="131" spans="14:16">
       <c r="N131">
         <v>241</v>
       </c>
     </row>
-    <row r="133" spans="14:14">
+    <row r="132" spans="14:16">
+      <c r="P132">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="133" spans="14:16">
       <c r="N133">
         <v>252</v>
       </c>
     </row>
-    <row r="135" spans="14:14">
+    <row r="134" spans="14:16">
+      <c r="P134">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="135" spans="14:16">
       <c r="N135">
         <v>248</v>
       </c>
     </row>
-    <row r="137" spans="14:14">
+    <row r="136" spans="14:16">
+      <c r="P136">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="137" spans="14:16">
       <c r="N137">
         <v>232</v>
       </c>
     </row>
-    <row r="139" spans="14:14">
+    <row r="138" spans="14:16">
+      <c r="P138">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="139" spans="14:16">
       <c r="N139">
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="14:14">
+    <row r="140" spans="14:16">
+      <c r="P140">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="141" spans="14:16">
       <c r="N141">
         <v>244</v>
       </c>
     </row>
-    <row r="143" spans="14:14">
+    <row r="142" spans="14:16">
+      <c r="P142">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="143" spans="14:16">
       <c r="N143">
         <v>245</v>
       </c>
     </row>
-    <row r="145" spans="14:14">
+    <row r="144" spans="14:16">
+      <c r="P144">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="145" spans="14:16">
       <c r="N145">
         <v>230</v>
       </c>
     </row>
-    <row r="147" spans="14:14">
+    <row r="146" spans="14:16">
+      <c r="P146">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="147" spans="14:16">
       <c r="N147">
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="14:14">
+    <row r="148" spans="14:16">
+      <c r="P148">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="149" spans="14:16">
       <c r="N149">
         <v>247</v>
       </c>
     </row>
-    <row r="151" spans="14:14">
+    <row r="150" spans="14:16">
+      <c r="P150">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="151" spans="14:16">
       <c r="N151">
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="14:14">
+    <row r="152" spans="14:16">
+      <c r="P152">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="153" spans="14:16">
       <c r="N153">
         <v>258</v>
       </c>
     </row>
-    <row r="155" spans="14:14">
+    <row r="154" spans="14:16">
+      <c r="P154">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="155" spans="14:16">
       <c r="N155">
         <v>253</v>
       </c>
     </row>
-    <row r="157" spans="14:14">
+    <row r="156" spans="14:16">
+      <c r="P156">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="157" spans="14:16">
       <c r="N157">
         <v>236</v>
       </c>
     </row>
-    <row r="159" spans="14:14">
+    <row r="158" spans="14:16">
+      <c r="P158">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="159" spans="14:16">
       <c r="N159">
         <v>249</v>
       </c>
     </row>
-    <row r="161" spans="14:14">
+    <row r="160" spans="14:16">
+      <c r="P160">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="161" spans="14:16">
       <c r="N161">
         <v>232</v>
       </c>
     </row>
-    <row r="163" spans="14:14">
+    <row r="162" spans="14:16">
+      <c r="P162">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="163" spans="14:16">
       <c r="N163">
         <v>245</v>
       </c>
     </row>
-    <row r="165" spans="14:14">
+    <row r="164" spans="14:16">
+      <c r="P164">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="165" spans="14:16">
       <c r="N165">
         <v>234</v>
       </c>
     </row>
-    <row r="167" spans="14:14">
+    <row r="166" spans="14:16">
+      <c r="P166">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="167" spans="14:16">
       <c r="N167">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="14:14">
+    <row r="168" spans="14:16">
+      <c r="P168">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="169" spans="14:16">
       <c r="N169">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="14:14">
+    <row r="170" spans="14:16">
+      <c r="P170">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="171" spans="14:16">
       <c r="N171">
         <v>245</v>
       </c>
     </row>
-    <row r="173" spans="14:14">
+    <row r="172" spans="14:16">
+      <c r="P172">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="173" spans="14:16">
       <c r="N173">
         <v>250</v>
       </c>
     </row>
-    <row r="175" spans="14:14">
+    <row r="174" spans="14:16">
+      <c r="P174">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="175" spans="14:16">
       <c r="N175">
         <v>217</v>
       </c>
     </row>
-    <row r="177" spans="14:14">
+    <row r="176" spans="14:16">
+      <c r="P176">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="177" spans="14:16">
       <c r="N177">
         <v>252</v>
       </c>
     </row>
-    <row r="179" spans="14:14">
+    <row r="178" spans="14:16">
+      <c r="P178">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="179" spans="14:16">
       <c r="N179">
         <v>222</v>
       </c>
     </row>
-    <row r="181" spans="14:14">
+    <row r="180" spans="14:16">
+      <c r="P180">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="181" spans="14:16">
       <c r="N181">
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="14:14">
+    <row r="182" spans="14:16">
+      <c r="P182">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="183" spans="14:16">
       <c r="N183">
         <v>252</v>
       </c>
     </row>
-    <row r="185" spans="14:14">
+    <row r="184" spans="14:16">
+      <c r="P184">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="185" spans="14:16">
       <c r="N185">
         <v>248</v>
       </c>
     </row>
-    <row r="187" spans="14:14">
+    <row r="186" spans="14:16">
+      <c r="P186">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="187" spans="14:16">
       <c r="N187">
         <v>230</v>
       </c>
     </row>
-    <row r="189" spans="14:14">
+    <row r="188" spans="14:16">
+      <c r="P188">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="189" spans="14:16">
       <c r="N189">
         <v>230</v>
       </c>
     </row>
-    <row r="191" spans="14:14">
+    <row r="190" spans="14:16">
+      <c r="P190">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="191" spans="14:16">
       <c r="N191">
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="14:14">
+    <row r="192" spans="14:16">
+      <c r="P192">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="193" spans="14:16">
       <c r="N193">
         <v>253</v>
       </c>
     </row>
-    <row r="195" spans="14:14">
+    <row r="194" spans="14:16">
+      <c r="P194">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="195" spans="14:16">
       <c r="N195">
         <v>239</v>
       </c>
     </row>
-    <row r="197" spans="14:14">
+    <row r="196" spans="14:16">
+      <c r="P196">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="197" spans="14:16">
       <c r="N197">
         <v>256</v>
       </c>
     </row>
-    <row r="199" spans="14:14">
+    <row r="198" spans="14:16">
+      <c r="P198">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="199" spans="14:16">
       <c r="N199">
         <v>257</v>
       </c>
     </row>
-    <row r="201" spans="14:14">
+    <row r="200" spans="14:16">
+      <c r="P200">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="201" spans="14:16">
       <c r="N201">
         <v>225</v>
       </c>
     </row>
-    <row r="203" spans="14:14">
+    <row r="202" spans="14:16">
+      <c r="P202">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="203" spans="14:16">
       <c r="N203">
         <v>247</v>
+      </c>
+    </row>
+    <row r="204" spans="14:16">
+      <c r="P204">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -5286,4 +5806,1539 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="J1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="10:16">
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="10:16">
+      <c r="J3">
+        <v>1000</v>
+      </c>
+      <c r="K3">
+        <v>481.4</v>
+      </c>
+      <c r="L3">
+        <v>6.12</v>
+      </c>
+      <c r="M3">
+        <v>535.20000000000005</v>
+      </c>
+      <c r="N3">
+        <v>10.23</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="0">K3/M3</f>
+        <v>0.89947683109118071</v>
+      </c>
+    </row>
+    <row r="4" spans="10:16">
+      <c r="J4">
+        <v>2000</v>
+      </c>
+      <c r="K4">
+        <v>2139.1999999999998</v>
+      </c>
+      <c r="L4">
+        <v>15.16</v>
+      </c>
+      <c r="M4">
+        <v>2719.2</v>
+      </c>
+      <c r="N4">
+        <v>31.84</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.78670197116799057</v>
+      </c>
+    </row>
+    <row r="5" spans="10:16">
+      <c r="J5">
+        <v>3000</v>
+      </c>
+      <c r="K5">
+        <v>5655</v>
+      </c>
+      <c r="L5">
+        <v>48.73</v>
+      </c>
+      <c r="M5">
+        <v>7796.2</v>
+      </c>
+      <c r="N5">
+        <v>29.48</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.72535337728637028</v>
+      </c>
+    </row>
+    <row r="6" spans="10:16">
+      <c r="J6">
+        <v>4000</v>
+      </c>
+      <c r="K6">
+        <v>11626.4</v>
+      </c>
+      <c r="L6">
+        <v>120.09</v>
+      </c>
+      <c r="M6">
+        <v>16915</v>
+      </c>
+      <c r="N6">
+        <v>40.14</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.68734259532958908</v>
+      </c>
+    </row>
+    <row r="7" spans="10:16">
+      <c r="J7">
+        <v>5000</v>
+      </c>
+      <c r="K7">
+        <v>20279.8</v>
+      </c>
+      <c r="L7">
+        <v>33.65</v>
+      </c>
+      <c r="M7">
+        <v>31284.799999999999</v>
+      </c>
+      <c r="N7">
+        <v>64.569999999999993</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.64823172914642258</v>
+      </c>
+    </row>
+    <row r="8" spans="10:16">
+      <c r="J8">
+        <v>6000</v>
+      </c>
+      <c r="K8">
+        <v>32804.6</v>
+      </c>
+      <c r="L8">
+        <v>232.71</v>
+      </c>
+      <c r="M8">
+        <v>52027.4</v>
+      </c>
+      <c r="N8">
+        <v>109.6</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0.63052545389544734</v>
+      </c>
+    </row>
+    <row r="9" spans="10:16">
+      <c r="J9">
+        <v>7000</v>
+      </c>
+      <c r="K9">
+        <v>49707.8</v>
+      </c>
+      <c r="L9">
+        <v>421.68</v>
+      </c>
+      <c r="M9">
+        <v>81267.399999999994</v>
+      </c>
+      <c r="N9">
+        <v>349.61</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.6116573189249318</v>
+      </c>
+    </row>
+    <row r="10" spans="10:16">
+      <c r="J10">
+        <v>8000</v>
+      </c>
+      <c r="K10">
+        <v>70965.399999999994</v>
+      </c>
+      <c r="L10">
+        <v>437.87</v>
+      </c>
+      <c r="M10">
+        <v>118798</v>
+      </c>
+      <c r="N10">
+        <v>311.64</v>
+      </c>
+      <c r="P10">
+        <f>K10/M10</f>
+        <v>0.5973619084496371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="3">
+        <v>41275</v>
+      </c>
+      <c r="B1" s="4">
+        <v>31065</v>
+      </c>
+      <c r="C1" s="5">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4">
+        <v>259692</v>
+      </c>
+      <c r="E1" s="4">
+        <v>1189076</v>
+      </c>
+      <c r="F1" s="4">
+        <v>229983</v>
+      </c>
+      <c r="G1" s="4">
+        <v>281861</v>
+      </c>
+      <c r="H1" s="4">
+        <v>40217</v>
+      </c>
+      <c r="I1" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="J1" s="5">
+        <v>78.930000000000007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3">
+        <v>41306</v>
+      </c>
+      <c r="B2" s="4">
+        <v>43197</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45</v>
+      </c>
+      <c r="D2" s="4">
+        <v>203097</v>
+      </c>
+      <c r="E2" s="4">
+        <v>912654</v>
+      </c>
+      <c r="F2" s="4">
+        <v>196042</v>
+      </c>
+      <c r="G2" s="4">
+        <v>233284</v>
+      </c>
+      <c r="H2" s="4">
+        <v>52377</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1.04</v>
+      </c>
+      <c r="J2" s="5">
+        <v>72.319999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3">
+        <v>41334</v>
+      </c>
+      <c r="B3" s="4">
+        <v>60368</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45</v>
+      </c>
+      <c r="D3" s="4">
+        <v>265057</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2529113</v>
+      </c>
+      <c r="F3" s="4">
+        <v>246789</v>
+      </c>
+      <c r="G3" s="4">
+        <v>300580</v>
+      </c>
+      <c r="H3" s="4">
+        <v>69612</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1.07</v>
+      </c>
+      <c r="J3" s="5">
+        <v>84.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3">
+        <v>41365</v>
+      </c>
+      <c r="B4" s="4">
+        <v>58799</v>
+      </c>
+      <c r="C4" s="5">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4">
+        <v>266861</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2455763</v>
+      </c>
+      <c r="F4" s="4">
+        <v>255621</v>
+      </c>
+      <c r="G4" s="4">
+        <v>278149</v>
+      </c>
+      <c r="H4" s="4">
+        <v>73397</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.04</v>
+      </c>
+      <c r="J4" s="5">
+        <v>80.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="3">
+        <v>41395</v>
+      </c>
+      <c r="B5" s="4">
+        <v>94168</v>
+      </c>
+      <c r="C5" s="5">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4">
+        <v>286148</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3902610</v>
+      </c>
+      <c r="F5" s="4">
+        <v>255357</v>
+      </c>
+      <c r="G5" s="4">
+        <v>293238</v>
+      </c>
+      <c r="H5" s="4">
+        <v>104511</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J5" s="5">
+        <v>82.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="3">
+        <v>41426</v>
+      </c>
+      <c r="B6" s="4">
+        <v>28050</v>
+      </c>
+      <c r="C6" s="5">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4">
+        <v>274405</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1307781</v>
+      </c>
+      <c r="F6" s="4">
+        <v>250900</v>
+      </c>
+      <c r="G6" s="4">
+        <v>285340</v>
+      </c>
+      <c r="H6" s="4">
+        <v>37354</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J6" s="5">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="3">
+        <v>41456</v>
+      </c>
+      <c r="B7" s="4">
+        <v>19987</v>
+      </c>
+      <c r="C7" s="5">
+        <v>35</v>
+      </c>
+      <c r="D7" s="4">
+        <v>267532</v>
+      </c>
+      <c r="E7" s="4">
+        <v>747745</v>
+      </c>
+      <c r="F7" s="4">
+        <v>238544</v>
+      </c>
+      <c r="G7" s="4">
+        <v>273697</v>
+      </c>
+      <c r="H7" s="4">
+        <v>27649</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J7" s="5">
+        <v>76.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="3">
+        <v>41487</v>
+      </c>
+      <c r="B8" s="4">
+        <v>23114</v>
+      </c>
+      <c r="C8" s="5">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4">
+        <v>298123</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1022083</v>
+      </c>
+      <c r="F8" s="4">
+        <v>260617</v>
+      </c>
+      <c r="G8" s="4">
+        <v>305740</v>
+      </c>
+      <c r="H8" s="4">
+        <v>28278</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J8" s="5">
+        <v>85.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="3">
+        <v>41518</v>
+      </c>
+      <c r="B9" s="6">
+        <v>50830</v>
+      </c>
+      <c r="C9" s="7">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6">
+        <v>290808</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2155175</v>
+      </c>
+      <c r="F9" s="6">
+        <v>267533</v>
+      </c>
+      <c r="G9" s="6">
+        <v>305323</v>
+      </c>
+      <c r="H9" s="6">
+        <v>56684</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J9" s="5">
+        <v>88.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="3">
+        <v>41548</v>
+      </c>
+      <c r="B10" s="4">
+        <v>40193</v>
+      </c>
+      <c r="C10" s="5">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4">
+        <v>247323</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1454128</v>
+      </c>
+      <c r="F10" s="4">
+        <v>282097</v>
+      </c>
+      <c r="G10" s="4">
+        <v>294255</v>
+      </c>
+      <c r="H10" s="4">
+        <v>41987</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="J10" s="5">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="3">
+        <v>41579</v>
+      </c>
+      <c r="B11" s="4">
+        <v>52144</v>
+      </c>
+      <c r="C11" s="5">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4">
+        <v>288281</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1743118</v>
+      </c>
+      <c r="F11" s="4">
+        <v>284133</v>
+      </c>
+      <c r="G11" s="4">
+        <v>300983</v>
+      </c>
+      <c r="H11" s="4">
+        <v>53859</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J11" s="5">
+        <v>87.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="3">
+        <v>41609</v>
+      </c>
+      <c r="B12" s="4">
+        <v>44591</v>
+      </c>
+      <c r="C12" s="5">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4">
+        <v>244663</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1405118</v>
+      </c>
+      <c r="F12" s="4">
+        <v>251138</v>
+      </c>
+      <c r="G12" s="4">
+        <v>259117</v>
+      </c>
+      <c r="H12" s="4">
+        <v>46118</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="J12" s="5">
+        <v>72.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17">
+      <c r="A13" s="8"/>
+      <c r="J13">
+        <f>AVERAGE(J1:J12)</f>
+        <v>81.096666666666678</v>
+      </c>
+      <c r="K13">
+        <f>STDEV(J1:J12)</f>
+        <v>5.2038662782996497</v>
+      </c>
+      <c r="L13">
+        <f>MIN(J1:J12)</f>
+        <v>72.319999999999993</v>
+      </c>
+      <c r="M13">
+        <f>MAX(J1:J12)</f>
+        <v>88.35</v>
+      </c>
+      <c r="N13">
+        <f>ABS(M13-L13)</f>
+        <v>16.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" ht="18">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3">
+        <v>41275</v>
+      </c>
+      <c r="B16" s="4">
+        <v>82739</v>
+      </c>
+      <c r="C16" s="5">
+        <v>120</v>
+      </c>
+      <c r="D16" s="4">
+        <v>601868</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1670641</v>
+      </c>
+      <c r="F16" s="4">
+        <v>344030</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1448128</v>
+      </c>
+      <c r="H16" s="4">
+        <v>455972</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1.75</v>
+      </c>
+      <c r="J16" s="5">
+        <v>76.989999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="3">
+        <v>41306</v>
+      </c>
+      <c r="B17" s="4">
+        <v>154467</v>
+      </c>
+      <c r="C17" s="5">
+        <v>115</v>
+      </c>
+      <c r="D17" s="4">
+        <v>504389</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3362768</v>
+      </c>
+      <c r="F17" s="4">
+        <v>269725</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1178271</v>
+      </c>
+      <c r="H17" s="4">
+        <v>550619</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="J17" s="5">
+        <v>69.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="3">
+        <v>41334</v>
+      </c>
+      <c r="B18" s="4">
+        <v>204474</v>
+      </c>
+      <c r="C18" s="5">
+        <v>147</v>
+      </c>
+      <c r="D18" s="4">
+        <v>750774</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3434836</v>
+      </c>
+      <c r="F18" s="4">
+        <v>449952</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1348127</v>
+      </c>
+      <c r="H18" s="4">
+        <v>387864</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1.67</v>
+      </c>
+      <c r="J18" s="5">
+        <v>71.680000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="3">
+        <v>41365</v>
+      </c>
+      <c r="B19" s="4">
+        <v>392644</v>
+      </c>
+      <c r="C19" s="5">
+        <v>148</v>
+      </c>
+      <c r="D19" s="4">
+        <v>790634</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5375478</v>
+      </c>
+      <c r="F19" s="4">
+        <v>499238</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1367823</v>
+      </c>
+      <c r="H19" s="4">
+        <v>618888</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1.58</v>
+      </c>
+      <c r="J19" s="5">
+        <v>75.150000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="3">
+        <v>41395</v>
+      </c>
+      <c r="B20" s="4">
+        <v>295232</v>
+      </c>
+      <c r="C20" s="5">
+        <v>139</v>
+      </c>
+      <c r="D20" s="4">
+        <v>851918</v>
+      </c>
+      <c r="E20" s="4">
+        <v>4186113</v>
+      </c>
+      <c r="F20" s="4">
+        <v>548855</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1377309</v>
+      </c>
+      <c r="H20" s="4">
+        <v>717113</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1.55</v>
+      </c>
+      <c r="J20" s="5">
+        <v>73.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="3">
+        <v>41426</v>
+      </c>
+      <c r="B21" s="4">
+        <v>504595</v>
+      </c>
+      <c r="C21" s="5">
+        <v>115</v>
+      </c>
+      <c r="D21" s="4">
+        <v>722065</v>
+      </c>
+      <c r="E21" s="4">
+        <v>7663194</v>
+      </c>
+      <c r="F21" s="4">
+        <v>406622</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1348851</v>
+      </c>
+      <c r="H21" s="4">
+        <v>903648</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1.78</v>
+      </c>
+      <c r="J21" s="5">
+        <v>74.11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="3">
+        <v>41456</v>
+      </c>
+      <c r="B22" s="4">
+        <v>180082</v>
+      </c>
+      <c r="C22" s="5">
+        <v>129</v>
+      </c>
+      <c r="D22" s="4">
+        <v>826744</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3208650</v>
+      </c>
+      <c r="F22" s="4">
+        <v>518270</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1274331</v>
+      </c>
+      <c r="H22" s="4">
+        <v>298292</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="J22" s="5">
+        <v>67.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="3">
+        <v>41487</v>
+      </c>
+      <c r="B23" s="4">
+        <v>241449</v>
+      </c>
+      <c r="C23" s="5">
+        <v>121</v>
+      </c>
+      <c r="D23" s="4">
+        <v>808675</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4539863</v>
+      </c>
+      <c r="F23" s="4">
+        <v>448813</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1287586</v>
+      </c>
+      <c r="H23" s="4">
+        <v>355065</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="J23" s="5">
+        <v>68.459999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="3">
+        <v>41518</v>
+      </c>
+      <c r="B24" s="4">
+        <v>173461</v>
+      </c>
+      <c r="C24" s="5">
+        <v>135</v>
+      </c>
+      <c r="D24" s="4">
+        <v>717576</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3013799</v>
+      </c>
+      <c r="F24" s="4">
+        <v>342802</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1182882</v>
+      </c>
+      <c r="H24" s="4">
+        <v>351445</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2.09</v>
+      </c>
+      <c r="J24" s="5">
+        <v>64.989999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="3">
+        <v>41548</v>
+      </c>
+      <c r="B25" s="10">
+        <v>142468</v>
+      </c>
+      <c r="C25" s="5">
+        <v>140</v>
+      </c>
+      <c r="D25" s="4">
+        <v>800309</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3781799</v>
+      </c>
+      <c r="F25" s="4">
+        <v>477225</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1355864</v>
+      </c>
+      <c r="H25" s="4">
+        <v>288123</v>
+      </c>
+      <c r="I25" s="5">
+        <v>1.68</v>
+      </c>
+      <c r="J25" s="5">
+        <v>72.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="3">
+        <v>41579</v>
+      </c>
+      <c r="B26" s="4">
+        <v>294733</v>
+      </c>
+      <c r="C26" s="5">
+        <v>146</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1030671</v>
+      </c>
+      <c r="E26" s="4">
+        <v>8395043</v>
+      </c>
+      <c r="F26" s="4">
+        <v>769720</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1405593</v>
+      </c>
+      <c r="H26" s="4">
+        <v>403198</v>
+      </c>
+      <c r="I26" s="5">
+        <v>1.34</v>
+      </c>
+      <c r="J26" s="5">
+        <v>77.22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="3">
+        <v>41609</v>
+      </c>
+      <c r="B27" s="4">
+        <v>264593</v>
+      </c>
+      <c r="C27" s="5">
+        <v>134</v>
+      </c>
+      <c r="D27" s="4">
+        <v>865914</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4534049</v>
+      </c>
+      <c r="F27" s="4">
+        <v>608689</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1151032</v>
+      </c>
+      <c r="H27" s="4">
+        <v>440453</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1.42</v>
+      </c>
+      <c r="J27" s="5">
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="17">
+      <c r="A28" s="8"/>
+      <c r="J28">
+        <f>AVERAGE(J16:J27)</f>
+        <v>71.019166666666678</v>
+      </c>
+      <c r="K28">
+        <f>STDEV(J16:J27)</f>
+        <v>4.8612184374876328</v>
+      </c>
+      <c r="L28">
+        <f>MIN(J16:J27)</f>
+        <v>61.2</v>
+      </c>
+      <c r="M28">
+        <f>MAX(J16:J27)</f>
+        <v>77.22</v>
+      </c>
+      <c r="N28">
+        <f>ABS(M28-L28)</f>
+        <v>16.019999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" ht="18">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:14" ht="18">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" ht="18">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="3">
+        <v>41275</v>
+      </c>
+      <c r="B33" s="4">
+        <v>29392</v>
+      </c>
+      <c r="C33" s="5">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4">
+        <v>609921</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1215124</v>
+      </c>
+      <c r="F33" s="4">
+        <v>240904</v>
+      </c>
+      <c r="G33" s="4">
+        <v>651243</v>
+      </c>
+      <c r="H33" s="4">
+        <v>59315</v>
+      </c>
+      <c r="I33" s="5">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="J33" s="5">
+        <v>88.24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="3">
+        <v>41306</v>
+      </c>
+      <c r="B34" s="4">
+        <v>18201</v>
+      </c>
+      <c r="C34" s="5">
+        <v>18</v>
+      </c>
+      <c r="D34" s="4">
+        <v>311975</v>
+      </c>
+      <c r="E34" s="4">
+        <v>436083</v>
+      </c>
+      <c r="F34" s="4">
+        <v>106844</v>
+      </c>
+      <c r="G34" s="4">
+        <v>383896</v>
+      </c>
+      <c r="H34" s="4">
+        <v>56734</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2.92</v>
+      </c>
+      <c r="J34" s="5">
+        <v>57.59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="3">
+        <v>41334</v>
+      </c>
+      <c r="B35" s="4">
+        <v>23070</v>
+      </c>
+      <c r="C35" s="5">
+        <v>16</v>
+      </c>
+      <c r="D35" s="4">
+        <v>427662</v>
+      </c>
+      <c r="E35" s="4">
+        <v>580618</v>
+      </c>
+      <c r="F35" s="4">
+        <v>166924</v>
+      </c>
+      <c r="G35" s="4">
+        <v>562392</v>
+      </c>
+      <c r="H35" s="4">
+        <v>43387</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2.56</v>
+      </c>
+      <c r="J35" s="5">
+        <v>76.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="3">
+        <v>41365</v>
+      </c>
+      <c r="B36" s="4">
+        <v>9851</v>
+      </c>
+      <c r="C36" s="5">
+        <v>14</v>
+      </c>
+      <c r="D36" s="4">
+        <v>122480</v>
+      </c>
+      <c r="E36" s="4">
+        <v>215113</v>
+      </c>
+      <c r="F36" s="4">
+        <v>112712</v>
+      </c>
+      <c r="G36" s="4">
+        <v>674342</v>
+      </c>
+      <c r="H36" s="4">
+        <v>25011</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J36" s="5">
+        <v>94.41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="3">
+        <v>41395</v>
+      </c>
+      <c r="B37" s="4">
+        <v>22885</v>
+      </c>
+      <c r="C37" s="5">
+        <v>12</v>
+      </c>
+      <c r="D37" s="4">
+        <v>223973</v>
+      </c>
+      <c r="E37" s="4">
+        <v>895838</v>
+      </c>
+      <c r="F37" s="4">
+        <v>189236</v>
+      </c>
+      <c r="G37" s="4">
+        <v>485275</v>
+      </c>
+      <c r="H37" s="4">
+        <v>33000</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1.18</v>
+      </c>
+      <c r="J37" s="5">
+        <v>65.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="3">
+        <v>41426</v>
+      </c>
+      <c r="B38" s="4">
+        <v>23590</v>
+      </c>
+      <c r="C38" s="5">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4">
+        <v>303553</v>
+      </c>
+      <c r="E38" s="4">
+        <v>964880</v>
+      </c>
+      <c r="F38" s="4">
+        <v>226173</v>
+      </c>
+      <c r="G38" s="4">
+        <v>531018</v>
+      </c>
+      <c r="H38" s="4">
+        <v>27720</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1.34</v>
+      </c>
+      <c r="J38" s="5">
+        <v>74.349999999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="3">
+        <v>41456</v>
+      </c>
+      <c r="B39" s="4">
+        <v>13480</v>
+      </c>
+      <c r="C39" s="5">
+        <v>10</v>
+      </c>
+      <c r="D39" s="4">
+        <v>172888</v>
+      </c>
+      <c r="E39" s="4">
+        <v>572809</v>
+      </c>
+      <c r="F39" s="4">
+        <v>150954</v>
+      </c>
+      <c r="G39" s="4">
+        <v>623161</v>
+      </c>
+      <c r="H39" s="4">
+        <v>15338</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J39" s="5">
+        <v>84.43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="3">
+        <v>41487</v>
+      </c>
+      <c r="B40" s="4">
+        <v>16588</v>
+      </c>
+      <c r="C40" s="5">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4">
+        <v>167149</v>
+      </c>
+      <c r="E40" s="4">
+        <v>505177</v>
+      </c>
+      <c r="F40" s="4">
+        <v>167278</v>
+      </c>
+      <c r="G40" s="4">
+        <v>427233</v>
+      </c>
+      <c r="H40" s="4">
+        <v>22471</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5">
+        <v>57.89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="3">
+        <v>41518</v>
+      </c>
+      <c r="B41" s="4">
+        <v>13546</v>
+      </c>
+      <c r="C41" s="5">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4">
+        <v>157176</v>
+      </c>
+      <c r="E41" s="4">
+        <v>438497</v>
+      </c>
+      <c r="F41" s="4">
+        <v>137557</v>
+      </c>
+      <c r="G41" s="4">
+        <v>455443</v>
+      </c>
+      <c r="H41" s="4">
+        <v>22892</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J41" s="5">
+        <v>63.77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="3">
+        <v>41548</v>
+      </c>
+      <c r="B42" s="4">
+        <v>10592</v>
+      </c>
+      <c r="C42" s="5">
+        <v>11</v>
+      </c>
+      <c r="D42" s="4">
+        <v>129192</v>
+      </c>
+      <c r="E42" s="4">
+        <v>382077</v>
+      </c>
+      <c r="F42" s="4">
+        <v>107286</v>
+      </c>
+      <c r="G42" s="4">
+        <v>600688</v>
+      </c>
+      <c r="H42" s="4">
+        <v>26318</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="J42" s="5">
+        <v>81.39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="3">
+        <v>41579</v>
+      </c>
+      <c r="B43" s="4">
+        <v>19245</v>
+      </c>
+      <c r="C43" s="5">
+        <v>9</v>
+      </c>
+      <c r="D43" s="4">
+        <v>150757</v>
+      </c>
+      <c r="E43" s="4">
+        <v>537774</v>
+      </c>
+      <c r="F43" s="4">
+        <v>121227</v>
+      </c>
+      <c r="G43" s="4">
+        <v>409866</v>
+      </c>
+      <c r="H43" s="4">
+        <v>19834</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1.24</v>
+      </c>
+      <c r="J43" s="5">
+        <v>57.38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="3">
+        <v>41609</v>
+      </c>
+      <c r="B44" s="4">
+        <v>18812</v>
+      </c>
+      <c r="C44" s="5">
+        <v>11</v>
+      </c>
+      <c r="D44" s="4">
+        <v>151858</v>
+      </c>
+      <c r="E44" s="4">
+        <v>451141</v>
+      </c>
+      <c r="F44" s="4">
+        <v>116393</v>
+      </c>
+      <c r="G44" s="4">
+        <v>824030</v>
+      </c>
+      <c r="H44" s="4">
+        <v>25413</v>
+      </c>
+      <c r="I44" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J44" s="5">
+        <v>111.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="J45">
+        <f>AVERAGE(J33:J44)</f>
+        <v>76.087499999999991</v>
+      </c>
+      <c r="K45">
+        <f>STDEV(J33:J44)</f>
+        <v>16.87035006642235</v>
+      </c>
+      <c r="L45">
+        <f>MIN(J33:J44)</f>
+        <v>57.38</v>
+      </c>
+      <c r="M45">
+        <f>MAX(J33:J44)</f>
+        <v>111.65</v>
+      </c>
+      <c r="N45">
+        <f>ABS(M45-L45)</f>
+        <v>54.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
graphing and more content to main
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17660" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
   <si>
     <t>Local</t>
   </si>
@@ -79,9 +79,6 @@
     <t>144 cores 1Gbit</t>
   </si>
   <si>
-    <t>8 cores 1Gbit</t>
-  </si>
-  <si>
     <t>Computation</t>
   </si>
   <si>
@@ -106,13 +103,7 @@
     <t>n=100</t>
   </si>
   <si>
-    <t>Aparapi small kernel small data</t>
-  </si>
-  <si>
     <t>Aparapi</t>
-  </si>
-  <si>
-    <t>Original</t>
   </si>
   <si>
     <t>2 Devices 1Gbit</t>
@@ -121,10 +112,19 @@
     <t>Single Device</t>
   </si>
   <si>
-    <t>Aparapi &gt;100lines</t>
+    <t>Aparapi 1000lines</t>
   </si>
   <si>
-    <t>Aparapi &gt;1000lines</t>
+    <t>Aparapi 1 lines small data</t>
+  </si>
+  <si>
+    <t>8 cores 10Gbit</t>
+  </si>
+  <si>
+    <t>Original like Aparapi</t>
+  </si>
+  <si>
+    <t>Original by hand</t>
   </si>
 </sst>
 </file>
@@ -213,8 +213,134 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="619">
+  <cellStyleXfs count="745">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -848,7 +974,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="619">
+  <cellStyles count="745">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1158,6 +1284,69 @@
     <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1467,6 +1656,69 @@
     <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1798,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView showRuler="0" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1889,7 +2141,7 @@
         <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>12</v>
@@ -1904,7 +2156,7 @@
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -2513,7 +2765,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -2585,7 +2837,7 @@
         <v>15</v>
       </c>
       <c r="J35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O35" t="s">
         <v>12</v>
@@ -2600,7 +2852,7 @@
         <v>15</v>
       </c>
       <c r="W35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -3208,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S46"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29:P37"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3228,40 +3480,40 @@
     </row>
     <row r="3" spans="1:16">
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
       <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3737,40 +3989,40 @@
     </row>
     <row r="29" spans="1:19">
       <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>21</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>22</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-      <c r="G29" t="s">
-        <v>25</v>
-      </c>
       <c r="K29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" t="s">
         <v>20</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>21</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>22</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>23</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>24</v>
-      </c>
-      <c r="P29" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -4275,23 +4527,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P204"/>
+  <dimension ref="A1:P203"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -4302,10 +4554,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -4313,20 +4565,24 @@
         <v>1000</v>
       </c>
       <c r="B3">
-        <v>224.2</v>
+        <v>138.6</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>75.7</v>
       </c>
       <c r="E3">
-        <v>206.37</v>
+        <v>110.53700000000001</v>
       </c>
       <c r="F3">
-        <v>49.902700000000003</v>
+        <v>45.021500000000003</v>
       </c>
       <c r="G3">
+        <f>E3/B3</f>
+        <v>0.79752525252525264</v>
+      </c>
+      <c r="H3">
         <f>B3/E3</f>
-        <v>1.0863982167950768</v>
+        <v>1.2538787917168006</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -4334,23 +4590,30 @@
         <v>2000</v>
       </c>
       <c r="B4">
-        <v>1595.8</v>
+        <v>592.79999999999995</v>
       </c>
       <c r="C4">
-        <v>0.75</v>
+        <v>3.43</v>
       </c>
       <c r="E4">
-        <v>1290.69</v>
+        <v>580.35199999999998</v>
       </c>
       <c r="F4">
-        <v>2.7359499999999999</v>
+        <v>1.3360700000000001</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G10" si="0">B4/E4</f>
-        <v>1.2363929371111575</v>
+        <f t="shared" ref="G4:G10" si="0">E4/B4</f>
+        <v>0.97900134952766538</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H10" si="1">B4/E4</f>
+        <v>1.0214490516100574</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4358,34 +4621,35 @@
         <v>3000</v>
       </c>
       <c r="B5">
-        <v>5312.8</v>
+        <v>1933.2</v>
       </c>
       <c r="C5">
-        <v>2.04</v>
+        <v>17.77</v>
       </c>
       <c r="E5">
-        <v>4375.71</v>
+        <v>1902.77</v>
       </c>
       <c r="F5">
-        <v>44.787300000000002</v>
+        <v>2.1463000000000001</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.2141572453384708</v>
+        <v>0.98425925925925928</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.0159924741298212</v>
       </c>
       <c r="I5">
         <f>AVERAGE(L:L)</f>
-        <v>199.87</v>
+        <v>31.42</v>
       </c>
       <c r="J5">
         <f>STDEV(L:L)</f>
-        <v>12.644841644007258</v>
+        <v>0.95536761130324721</v>
       </c>
       <c r="L5">
-        <v>214</v>
-      </c>
-      <c r="N5">
-        <v>250</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4393,26 +4657,27 @@
         <v>4000</v>
       </c>
       <c r="B6">
-        <v>12613.8</v>
+        <v>4596.6000000000004</v>
       </c>
       <c r="C6">
-        <v>77.900000000000006</v>
+        <v>32.340000000000003</v>
       </c>
       <c r="E6">
-        <v>11842</v>
+        <v>4508.82</v>
       </c>
       <c r="F6">
-        <v>70.101500000000001</v>
+        <v>27.655100000000001</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>1.0651748015537916</v>
-      </c>
-      <c r="L6">
-        <v>185</v>
+        <v>0.98090327633468199</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1.019468508390222</v>
       </c>
       <c r="P6">
-        <v>513</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4420,29 +4685,27 @@
         <v>5000</v>
       </c>
       <c r="B7">
-        <v>24732.400000000001</v>
+        <v>9466.6</v>
       </c>
       <c r="C7">
-        <v>38.81</v>
+        <v>289.66000000000003</v>
       </c>
       <c r="E7">
-        <v>24054.799999999999</v>
+        <v>9290.2999999999993</v>
       </c>
       <c r="F7">
-        <v>267.33499999999998</v>
+        <v>285.39600000000002</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.0281690140845072</v>
-      </c>
-      <c r="I7" t="s">
+        <v>0.98137662941288306</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1.0189767822352347</v>
+      </c>
+      <c r="L7">
         <v>32</v>
-      </c>
-      <c r="L7">
-        <v>192</v>
-      </c>
-      <c r="N7">
-        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4450,34 +4713,27 @@
         <v>6000</v>
       </c>
       <c r="B8">
-        <v>42903.8</v>
+        <v>16480.2</v>
       </c>
       <c r="C8">
-        <v>43.74</v>
+        <v>148.71</v>
       </c>
       <c r="E8">
-        <v>45420.800000000003</v>
+        <v>16213.1</v>
       </c>
       <c r="F8">
-        <v>276.31799999999998</v>
+        <v>161.62299999999999</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0.94458485979991547</v>
-      </c>
-      <c r="I8">
-        <f>AVERAGE(N:N)</f>
-        <v>242.82</v>
-      </c>
-      <c r="J8">
-        <f>STDEV(N:N)</f>
-        <v>13.155157992900799</v>
-      </c>
-      <c r="L8">
-        <v>178</v>
+        <v>0.98379267241902402</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.0164743324842258</v>
       </c>
       <c r="P8">
-        <v>510</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -4485,26 +4741,27 @@
         <v>7000</v>
       </c>
       <c r="B9">
-        <v>68075.199999999997</v>
+        <v>25800.2</v>
       </c>
       <c r="C9">
-        <v>222.12</v>
+        <v>176.48</v>
       </c>
       <c r="E9">
-        <v>82141.8</v>
+        <v>25749.3</v>
       </c>
       <c r="F9">
-        <v>521.84900000000005</v>
+        <v>71.982699999999994</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.82875223089827588</v>
+        <v>0.99802714707637918</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.0019767527660948</v>
       </c>
       <c r="L9">
-        <v>182</v>
-      </c>
-      <c r="N9">
-        <v>253</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4512,1289 +4769,1120 @@
         <v>8000</v>
       </c>
       <c r="B10">
-        <v>101557</v>
+        <v>39424.199999999997</v>
       </c>
       <c r="C10">
-        <v>316.44</v>
+        <v>218.29</v>
       </c>
       <c r="E10">
-        <v>155718</v>
+        <v>39366.870000000003</v>
       </c>
       <c r="F10">
-        <v>2521.4499999999998</v>
+        <v>195.92699999999999</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.6521853607161664</v>
+        <v>0.99854581703623679</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.0014563006914188</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10">
-        <v>214</v>
+        <v>29</v>
       </c>
       <c r="P10">
-        <v>491</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:16">
+      <c r="G11">
+        <f>AVERAGE(G6:G10)</f>
+        <v>0.98852910845584108</v>
+      </c>
       <c r="I11">
         <f>AVERAGE(P:P)</f>
-        <v>500.69</v>
+        <v>340.16</v>
       </c>
       <c r="J11">
         <f>STDEV(P:P)</f>
-        <v>15.120188524290995</v>
+        <v>2.5454256852620794</v>
       </c>
       <c r="L11">
-        <v>194</v>
-      </c>
-      <c r="N11">
-        <v>220</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="L12">
-        <v>182</v>
-      </c>
       <c r="P12">
-        <v>477</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="L13">
-        <v>198</v>
-      </c>
-      <c r="N13">
-        <v>253</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="L14">
-        <v>195</v>
+      <c r="A14" t="s">
+        <v>33</v>
       </c>
       <c r="P14">
-        <v>475</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:16">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
       <c r="L15">
-        <v>215</v>
-      </c>
-      <c r="N15">
-        <v>229</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="L16">
-        <v>200</v>
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>165.55</v>
+      </c>
+      <c r="C16">
+        <v>49.591999999999999</v>
+      </c>
+      <c r="D16">
+        <f>B16/B3</f>
+        <v>1.1944444444444446</v>
       </c>
       <c r="P16">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="17" spans="12:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>1007.89</v>
+      </c>
+      <c r="C17">
+        <v>2.9514900000000002</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D23" si="2">B17/B4</f>
+        <v>1.7002192982456141</v>
+      </c>
       <c r="L17">
-        <v>208</v>
-      </c>
-      <c r="N17">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="12:16">
-      <c r="L18">
-        <v>210</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <v>3000</v>
+      </c>
+      <c r="B18">
+        <v>3343.29</v>
+      </c>
+      <c r="C18">
+        <v>1.35182</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>1.7294072004965859</v>
       </c>
       <c r="P18">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="19" spans="12:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <v>4000</v>
+      </c>
+      <c r="B19">
+        <v>8161.56</v>
+      </c>
+      <c r="C19">
+        <v>334.51400000000001</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.7755645477091764</v>
+      </c>
       <c r="L19">
-        <v>196</v>
-      </c>
-      <c r="N19">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="12:16">
-      <c r="L20">
-        <v>202</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <v>5000</v>
+      </c>
+      <c r="B20">
+        <v>16789</v>
+      </c>
+      <c r="C20">
+        <v>60.207700000000003</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>1.7734984049183444</v>
       </c>
       <c r="P20">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="21" spans="12:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>6000</v>
+      </c>
+      <c r="B21">
+        <v>29125.200000000001</v>
+      </c>
+      <c r="C21">
+        <v>121.864</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>1.7672843776167764</v>
+      </c>
       <c r="L21">
-        <v>192</v>
-      </c>
-      <c r="N21">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="12:16">
-      <c r="L22">
-        <v>211</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <v>7000</v>
+      </c>
+      <c r="B22">
+        <v>46678.6</v>
+      </c>
+      <c r="C22">
+        <v>77.928200000000004</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>1.8092340369454498</v>
       </c>
       <c r="P22">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="23" spans="12:16">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>8000</v>
+      </c>
+      <c r="B23">
+        <v>69185.3</v>
+      </c>
+      <c r="C23">
+        <v>219.64699999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1.7548942020383422</v>
+      </c>
       <c r="L23">
-        <v>185</v>
-      </c>
-      <c r="N23">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="12:16">
-      <c r="L24">
-        <v>208</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="P24">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="25" spans="12:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="L25">
-        <v>197</v>
-      </c>
-      <c r="N25">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="12:16">
-      <c r="L26">
-        <v>211</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="P26">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="27" spans="12:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="L27">
-        <v>199</v>
-      </c>
-      <c r="N27">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="12:16">
-      <c r="L28">
-        <v>211</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="P28">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="29" spans="12:16">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="L29">
-        <v>185</v>
-      </c>
-      <c r="N29">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="12:16">
-      <c r="L30">
-        <v>214</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="P30">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="31" spans="12:16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="L31">
-        <v>192</v>
-      </c>
-      <c r="N31">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="32" spans="12:16">
-      <c r="L32">
-        <v>193</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="P32">
-        <v>512</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" spans="12:16">
       <c r="L33">
-        <v>194</v>
-      </c>
-      <c r="N33">
-        <v>256</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="12:16">
-      <c r="L34">
-        <v>213</v>
-      </c>
       <c r="P34">
-        <v>481</v>
+        <v>339</v>
       </c>
     </row>
     <row r="35" spans="12:16">
       <c r="L35">
-        <v>210</v>
-      </c>
-      <c r="N35">
-        <v>257</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="12:16">
-      <c r="L36">
-        <v>197</v>
-      </c>
       <c r="P36">
-        <v>495</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="12:16">
       <c r="L37">
-        <v>209</v>
-      </c>
-      <c r="N37">
-        <v>270</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="12:16">
-      <c r="L38">
-        <v>186</v>
-      </c>
       <c r="P38">
-        <v>486</v>
+        <v>338</v>
       </c>
     </row>
     <row r="39" spans="12:16">
       <c r="L39">
-        <v>197</v>
-      </c>
-      <c r="N39">
-        <v>232</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="12:16">
-      <c r="L40">
-        <v>194</v>
-      </c>
       <c r="P40">
-        <v>496</v>
+        <v>339</v>
       </c>
     </row>
     <row r="41" spans="12:16">
       <c r="L41">
-        <v>203</v>
-      </c>
-      <c r="N41">
-        <v>243</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="12:16">
-      <c r="L42">
-        <v>214</v>
-      </c>
       <c r="P42">
-        <v>502</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="12:16">
       <c r="L43">
-        <v>208</v>
-      </c>
-      <c r="N43">
-        <v>235</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="12:16">
-      <c r="L44">
-        <v>187</v>
-      </c>
       <c r="P44">
-        <v>490</v>
+        <v>339</v>
       </c>
     </row>
     <row r="45" spans="12:16">
       <c r="L45">
-        <v>210</v>
-      </c>
-      <c r="N45">
-        <v>234</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="12:16">
-      <c r="L46">
-        <v>182</v>
-      </c>
       <c r="P46">
-        <v>506</v>
+        <v>341</v>
       </c>
     </row>
     <row r="47" spans="12:16">
       <c r="L47">
-        <v>197</v>
-      </c>
-      <c r="N47">
-        <v>232</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="12:16">
-      <c r="L48">
-        <v>193</v>
-      </c>
       <c r="P48">
-        <v>514</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="12:16">
       <c r="L49">
-        <v>214</v>
-      </c>
-      <c r="N49">
-        <v>246</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="12:16">
-      <c r="L50">
-        <v>188</v>
-      </c>
       <c r="P50">
-        <v>488</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="12:16">
       <c r="L51">
-        <v>224</v>
-      </c>
-      <c r="N51">
-        <v>258</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="12:16">
-      <c r="L52">
-        <v>213</v>
-      </c>
       <c r="P52">
-        <v>509</v>
+        <v>345</v>
       </c>
     </row>
     <row r="53" spans="12:16">
       <c r="L53">
-        <v>194</v>
-      </c>
-      <c r="N53">
-        <v>247</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="12:16">
-      <c r="L54">
-        <v>177</v>
-      </c>
       <c r="P54">
-        <v>489</v>
+        <v>339</v>
       </c>
     </row>
     <row r="55" spans="12:16">
       <c r="L55">
-        <v>178</v>
-      </c>
-      <c r="N55">
-        <v>248</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="12:16">
-      <c r="L56">
-        <v>214</v>
-      </c>
       <c r="P56">
-        <v>499</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="12:16">
       <c r="L57">
-        <v>190</v>
-      </c>
-      <c r="N57">
-        <v>247</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="12:16">
-      <c r="L58">
-        <v>223</v>
-      </c>
       <c r="P58">
-        <v>507</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="12:16">
       <c r="L59">
-        <v>202</v>
-      </c>
-      <c r="N59">
-        <v>251</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="12:16">
-      <c r="L60">
-        <v>209</v>
-      </c>
       <c r="P60">
-        <v>477</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="12:16">
       <c r="L61">
-        <v>187</v>
-      </c>
-      <c r="N61">
-        <v>277</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="12:16">
-      <c r="L62">
-        <v>220</v>
-      </c>
       <c r="P62">
-        <v>491</v>
+        <v>340</v>
       </c>
     </row>
     <row r="63" spans="12:16">
       <c r="L63">
-        <v>191</v>
-      </c>
-      <c r="N63">
-        <v>259</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="12:16">
-      <c r="L64">
-        <v>210</v>
-      </c>
       <c r="P64">
-        <v>509</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="12:16">
       <c r="L65">
-        <v>179</v>
-      </c>
-      <c r="N65">
-        <v>235</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="12:16">
-      <c r="L66">
-        <v>210</v>
-      </c>
       <c r="P66">
-        <v>520</v>
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="12:16">
       <c r="L67">
-        <v>193</v>
-      </c>
-      <c r="N67">
-        <v>238</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="12:16">
-      <c r="L68">
-        <v>182</v>
-      </c>
       <c r="P68">
-        <v>488</v>
+        <v>342</v>
       </c>
     </row>
     <row r="69" spans="12:16">
       <c r="L69">
-        <v>218</v>
-      </c>
-      <c r="N69">
-        <v>228</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="12:16">
-      <c r="L70">
-        <v>226</v>
-      </c>
       <c r="P70">
-        <v>477</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="12:16">
       <c r="L71">
-        <v>204</v>
-      </c>
-      <c r="N71">
-        <v>253</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="12:16">
-      <c r="L72">
-        <v>198</v>
-      </c>
       <c r="P72">
-        <v>486</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="12:16">
       <c r="L73">
-        <v>196</v>
-      </c>
-      <c r="N73">
-        <v>231</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="12:16">
-      <c r="L74">
-        <v>176</v>
-      </c>
       <c r="P74">
-        <v>485</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="12:16">
       <c r="L75">
-        <v>194</v>
-      </c>
-      <c r="N75">
-        <v>245</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="12:16">
-      <c r="L76">
-        <v>191</v>
-      </c>
       <c r="P76">
-        <v>488</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="12:16">
       <c r="L77">
-        <v>204</v>
-      </c>
-      <c r="N77">
-        <v>218</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="12:16">
-      <c r="L78">
-        <v>212</v>
-      </c>
       <c r="P78">
-        <v>513</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="12:16">
       <c r="L79">
-        <v>213</v>
-      </c>
-      <c r="N79">
-        <v>250</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="12:16">
-      <c r="L80">
-        <v>192</v>
-      </c>
       <c r="P80">
-        <v>519</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="12:16">
       <c r="L81">
-        <v>210</v>
-      </c>
-      <c r="N81">
-        <v>249</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="12:16">
-      <c r="L82">
-        <v>212</v>
-      </c>
       <c r="P82">
-        <v>489</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="12:16">
       <c r="L83">
-        <v>181</v>
-      </c>
-      <c r="N83">
-        <v>235</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="12:16">
-      <c r="L84">
-        <v>190</v>
-      </c>
       <c r="P84">
-        <v>509</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="12:16">
       <c r="L85">
-        <v>193</v>
-      </c>
-      <c r="N85">
-        <v>275</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="12:16">
-      <c r="L86">
-        <v>186</v>
-      </c>
       <c r="P86">
-        <v>483</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" spans="12:16">
       <c r="L87">
-        <v>195</v>
-      </c>
-      <c r="N87">
-        <v>232</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="12:16">
-      <c r="L88">
-        <v>214</v>
-      </c>
       <c r="P88">
-        <v>509</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="12:16">
       <c r="L89">
-        <v>207</v>
-      </c>
-      <c r="N89">
-        <v>220</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="12:16">
-      <c r="L90">
-        <v>207</v>
-      </c>
       <c r="P90">
-        <v>529</v>
+        <v>339</v>
       </c>
     </row>
     <row r="91" spans="12:16">
       <c r="L91">
-        <v>210</v>
-      </c>
-      <c r="N91">
-        <v>264</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="12:16">
-      <c r="L92">
-        <v>220</v>
-      </c>
       <c r="P92">
-        <v>509</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="12:16">
       <c r="L93">
-        <v>181</v>
-      </c>
-      <c r="N93">
-        <v>236</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="12:16">
-      <c r="L94">
-        <v>209</v>
-      </c>
       <c r="P94">
-        <v>490</v>
+        <v>343</v>
       </c>
     </row>
     <row r="95" spans="12:16">
       <c r="L95">
-        <v>220</v>
-      </c>
-      <c r="N95">
-        <v>230</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="12:16">
-      <c r="L96">
-        <v>195</v>
-      </c>
       <c r="P96">
-        <v>491</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="12:16">
       <c r="L97">
-        <v>197</v>
-      </c>
-      <c r="N97">
-        <v>250</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="12:16">
-      <c r="L98">
-        <v>209</v>
-      </c>
       <c r="P98">
-        <v>490</v>
+        <v>345</v>
       </c>
     </row>
     <row r="99" spans="12:16">
       <c r="L99">
-        <v>188</v>
-      </c>
-      <c r="N99">
-        <v>233</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="12:16">
-      <c r="L100">
-        <v>191</v>
-      </c>
       <c r="P100">
-        <v>510</v>
+        <v>336</v>
       </c>
     </row>
     <row r="101" spans="12:16">
       <c r="L101">
-        <v>177</v>
-      </c>
-      <c r="N101">
-        <v>233</v>
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="12:16">
-      <c r="L102">
-        <v>191</v>
-      </c>
       <c r="P102">
-        <v>493</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="12:16">
       <c r="L103">
-        <v>209</v>
-      </c>
-      <c r="N103">
-        <v>218</v>
+        <v>31</v>
       </c>
     </row>
     <row r="104" spans="12:16">
-      <c r="L104">
-        <v>216</v>
-      </c>
       <c r="P104">
-        <v>505</v>
+        <v>341</v>
       </c>
     </row>
     <row r="105" spans="12:16">
-      <c r="N105">
-        <v>249</v>
+      <c r="L105">
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="12:16">
       <c r="P106">
-        <v>525</v>
+        <v>343</v>
       </c>
     </row>
     <row r="107" spans="12:16">
-      <c r="N107">
-        <v>229</v>
+      <c r="L107">
+        <v>31</v>
       </c>
     </row>
     <row r="108" spans="12:16">
       <c r="P108">
-        <v>498</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109" spans="12:16">
-      <c r="N109">
-        <v>241</v>
+      <c r="L109">
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="12:16">
       <c r="P110">
-        <v>488</v>
+        <v>342</v>
       </c>
     </row>
     <row r="111" spans="12:16">
-      <c r="N111">
-        <v>253</v>
+      <c r="L111">
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="12:16">
       <c r="P112">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="113" spans="14:16">
-      <c r="N113">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="114" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="113" spans="12:16">
+      <c r="L113">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="12:16">
       <c r="P114">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="115" spans="14:16">
-      <c r="N115">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="116" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="115" spans="12:16">
+      <c r="L115">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="12:16">
       <c r="P116">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="117" spans="14:16">
-      <c r="N117">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="118" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="117" spans="12:16">
+      <c r="L117">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="12:16">
       <c r="P118">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="119" spans="14:16">
-      <c r="N119">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="120" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="119" spans="12:16">
+      <c r="L119">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="120" spans="12:16">
       <c r="P120">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="121" spans="14:16">
-      <c r="N121">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="122" spans="14:16">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="121" spans="12:16">
+      <c r="L121">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="12:16">
       <c r="P122">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="123" spans="14:16">
-      <c r="N123">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="124" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="123" spans="12:16">
+      <c r="L123">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" spans="12:16">
       <c r="P124">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="125" spans="14:16">
-      <c r="N125">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="126" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="125" spans="12:16">
+      <c r="L125">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="12:16">
       <c r="P126">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="127" spans="14:16">
-      <c r="N127">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="128" spans="14:16">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="127" spans="12:16">
+      <c r="L127">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="128" spans="12:16">
       <c r="P128">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="129" spans="14:16">
-      <c r="N129">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="130" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="129" spans="12:16">
+      <c r="L129">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="12:16">
       <c r="P130">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="131" spans="14:16">
-      <c r="N131">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="132" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="131" spans="12:16">
+      <c r="L131">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="12:16">
       <c r="P132">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="133" spans="14:16">
-      <c r="N133">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="134" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="12:16">
+      <c r="L133">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="12:16">
       <c r="P134">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="135" spans="14:16">
-      <c r="N135">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="136" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="135" spans="12:16">
+      <c r="L135">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136" spans="12:16">
       <c r="P136">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="137" spans="14:16">
-      <c r="N137">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="138" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="137" spans="12:16">
+      <c r="L137">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="138" spans="12:16">
       <c r="P138">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="139" spans="14:16">
-      <c r="N139">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="140" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="139" spans="12:16">
+      <c r="L139">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="140" spans="12:16">
       <c r="P140">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="141" spans="14:16">
-      <c r="N141">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="142" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="141" spans="12:16">
+      <c r="L141">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="142" spans="12:16">
       <c r="P142">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="143" spans="14:16">
-      <c r="N143">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="144" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="143" spans="12:16">
+      <c r="L143">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144" spans="12:16">
       <c r="P144">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="145" spans="14:16">
-      <c r="N145">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="146" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="145" spans="12:16">
+      <c r="L145">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="12:16">
       <c r="P146">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="147" spans="14:16">
-      <c r="N147">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="148" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="147" spans="12:16">
+      <c r="L147">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="148" spans="12:16">
       <c r="P148">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="149" spans="14:16">
-      <c r="N149">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="150" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="149" spans="12:16">
+      <c r="L149">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="12:16">
       <c r="P150">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="151" spans="14:16">
-      <c r="N151">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="152" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="151" spans="12:16">
+      <c r="L151">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="152" spans="12:16">
       <c r="P152">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="153" spans="14:16">
-      <c r="N153">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="154" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="153" spans="12:16">
+      <c r="L153">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="12:16">
       <c r="P154">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="155" spans="14:16">
-      <c r="N155">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="156" spans="14:16">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="155" spans="12:16">
+      <c r="L155">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="12:16">
       <c r="P156">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="157" spans="14:16">
-      <c r="N157">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="158" spans="14:16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="157" spans="12:16">
+      <c r="L157">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="158" spans="12:16">
       <c r="P158">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="159" spans="14:16">
-      <c r="N159">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="160" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="159" spans="12:16">
+      <c r="L159">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="160" spans="12:16">
       <c r="P160">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="161" spans="14:16">
-      <c r="N161">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="162" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="161" spans="12:16">
+      <c r="L161">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="162" spans="12:16">
       <c r="P162">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="163" spans="14:16">
-      <c r="N163">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="164" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="163" spans="12:16">
+      <c r="L163">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="164" spans="12:16">
       <c r="P164">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="165" spans="14:16">
-      <c r="N165">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="166" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="165" spans="12:16">
+      <c r="L165">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="166" spans="12:16">
       <c r="P166">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="167" spans="14:16">
-      <c r="N167">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="168" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="167" spans="12:16">
+      <c r="L167">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="168" spans="12:16">
       <c r="P168">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="169" spans="14:16">
-      <c r="N169">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="170" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="169" spans="12:16">
+      <c r="L169">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="170" spans="12:16">
       <c r="P170">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="171" spans="14:16">
-      <c r="N171">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="172" spans="14:16">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="171" spans="12:16">
+      <c r="L171">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="172" spans="12:16">
       <c r="P172">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="173" spans="14:16">
-      <c r="N173">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="174" spans="14:16">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="173" spans="12:16">
+      <c r="L173">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="174" spans="12:16">
       <c r="P174">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="175" spans="14:16">
-      <c r="N175">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="176" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="175" spans="12:16">
+      <c r="L175">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="176" spans="12:16">
       <c r="P176">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="177" spans="14:16">
-      <c r="N177">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="178" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="177" spans="12:16">
+      <c r="L177">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="178" spans="12:16">
       <c r="P178">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="179" spans="14:16">
-      <c r="N179">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="180" spans="14:16">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="179" spans="12:16">
+      <c r="L179">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="180" spans="12:16">
       <c r="P180">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="181" spans="14:16">
-      <c r="N181">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="182" spans="14:16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="181" spans="12:16">
+      <c r="L181">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="182" spans="12:16">
       <c r="P182">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="183" spans="14:16">
-      <c r="N183">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="184" spans="14:16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="183" spans="12:16">
+      <c r="L183">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="184" spans="12:16">
       <c r="P184">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="185" spans="14:16">
-      <c r="N185">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="186" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="185" spans="12:16">
+      <c r="L185">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="186" spans="12:16">
       <c r="P186">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="187" spans="14:16">
-      <c r="N187">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="188" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="187" spans="12:16">
+      <c r="L187">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="188" spans="12:16">
       <c r="P188">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="189" spans="14:16">
-      <c r="N189">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="190" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="189" spans="12:16">
+      <c r="L189">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="190" spans="12:16">
       <c r="P190">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="191" spans="14:16">
-      <c r="N191">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="192" spans="14:16">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="191" spans="12:16">
+      <c r="L191">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="192" spans="12:16">
       <c r="P192">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="193" spans="14:16">
-      <c r="N193">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="194" spans="14:16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="193" spans="12:16">
+      <c r="L193">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="194" spans="12:16">
       <c r="P194">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="195" spans="14:16">
-      <c r="N195">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="196" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="195" spans="12:16">
+      <c r="L195">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="196" spans="12:16">
       <c r="P196">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="197" spans="14:16">
-      <c r="N197">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="198" spans="14:16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="197" spans="12:16">
+      <c r="L197">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="12:16">
       <c r="P198">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="199" spans="14:16">
-      <c r="N199">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="200" spans="14:16">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="199" spans="12:16">
+      <c r="L199">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="200" spans="12:16">
       <c r="P200">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="201" spans="14:16">
-      <c r="N201">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="202" spans="14:16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="201" spans="12:16">
+      <c r="L201">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="202" spans="12:16">
       <c r="P202">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="203" spans="14:16">
-      <c r="N203">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="204" spans="14:16">
-      <c r="P204">
-        <v>503</v>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="203" spans="12:16">
+      <c r="L203">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5810,23 +5898,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J1:P10"/>
+  <dimension ref="J1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="10:16">
+    <row r="1" spans="10:17">
       <c r="J1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="10:16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="10:17">
       <c r="J3">
         <v>1000</v>
       </c>
@@ -5846,8 +5934,12 @@
         <f t="shared" ref="P3:P9" si="0">K3/M3</f>
         <v>0.89947683109118071</v>
       </c>
-    </row>
-    <row r="4" spans="10:16">
+      <c r="Q3">
+        <f>M3/K3</f>
+        <v>1.1117573743248859</v>
+      </c>
+    </row>
+    <row r="4" spans="10:17">
       <c r="J4">
         <v>2000</v>
       </c>
@@ -5867,8 +5959,12 @@
         <f t="shared" si="0"/>
         <v>0.78670197116799057</v>
       </c>
-    </row>
-    <row r="5" spans="10:16">
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q12" si="1">M4/K4</f>
+        <v>1.2711293941660433</v>
+      </c>
+    </row>
+    <row r="5" spans="10:17">
       <c r="J5">
         <v>3000</v>
       </c>
@@ -5888,8 +5984,12 @@
         <f t="shared" si="0"/>
         <v>0.72535337728637028</v>
       </c>
-    </row>
-    <row r="6" spans="10:16">
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>1.3786383731211318</v>
+      </c>
+    </row>
+    <row r="6" spans="10:17">
       <c r="J6">
         <v>4000</v>
       </c>
@@ -5909,8 +6009,12 @@
         <f t="shared" si="0"/>
         <v>0.68734259532958908</v>
       </c>
-    </row>
-    <row r="7" spans="10:16">
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>1.4548785522603729</v>
+      </c>
+    </row>
+    <row r="7" spans="10:17">
       <c r="J7">
         <v>5000</v>
       </c>
@@ -5930,8 +6034,12 @@
         <f t="shared" si="0"/>
         <v>0.64823172914642258</v>
       </c>
-    </row>
-    <row r="8" spans="10:16">
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>1.5426582116194441</v>
+      </c>
+    </row>
+    <row r="8" spans="10:17">
       <c r="J8">
         <v>6000</v>
       </c>
@@ -5951,8 +6059,12 @@
         <f t="shared" si="0"/>
         <v>0.63052545389544734</v>
       </c>
-    </row>
-    <row r="9" spans="10:16">
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>1.5859787956567069</v>
+      </c>
+    </row>
+    <row r="9" spans="10:17">
       <c r="J9">
         <v>7000</v>
       </c>
@@ -5972,8 +6084,12 @@
         <f t="shared" si="0"/>
         <v>0.6116573189249318</v>
       </c>
-    </row>
-    <row r="10" spans="10:16">
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>1.6349023694470484</v>
+      </c>
+    </row>
+    <row r="10" spans="10:17">
       <c r="J10">
         <v>8000</v>
       </c>
@@ -5993,9 +6109,64 @@
         <f>K10/M10</f>
         <v>0.5973619084496371</v>
       </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>1.6740270610748338</v>
+      </c>
+    </row>
+    <row r="11" spans="10:17">
+      <c r="J11">
+        <v>9000</v>
+      </c>
+      <c r="K11">
+        <v>98685.6</v>
+      </c>
+      <c r="L11">
+        <v>116.37</v>
+      </c>
+      <c r="M11">
+        <v>168573.4</v>
+      </c>
+      <c r="N11">
+        <v>243.48</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P12" si="2">K11/M11</f>
+        <v>0.58541620445455811</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>1.708186402068792</v>
+      </c>
+    </row>
+    <row r="12" spans="10:17">
+      <c r="J12">
+        <v>10000</v>
+      </c>
+      <c r="K12">
+        <v>131682.6</v>
+      </c>
+      <c r="L12">
+        <v>602.36</v>
+      </c>
+      <c r="M12">
+        <v>228206.6</v>
+      </c>
+      <c r="N12">
+        <v>1147.06</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>0.57703239082480529</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>1.7330049680064032</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
scalable speed and scheduling filled
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -213,8 +213,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="745">
+  <cellStyleXfs count="757">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -974,7 +986,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="745">
+  <cellStyles count="757">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1347,6 +1359,12 @@
     <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1719,6 +1737,12 @@
     <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4530,7 +4554,7 @@
   <dimension ref="A1:P203"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4576,14 +4600,6 @@
       <c r="F3">
         <v>45.021500000000003</v>
       </c>
-      <c r="G3">
-        <f>E3/B3</f>
-        <v>0.79752525252525264</v>
-      </c>
-      <c r="H3">
-        <f>B3/E3</f>
-        <v>1.2538787917168006</v>
-      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
@@ -4601,14 +4617,6 @@
       <c r="F4">
         <v>1.3360700000000001</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G10" si="0">E4/B4</f>
-        <v>0.97900134952766538</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H10" si="1">B4/E4</f>
-        <v>1.0214490516100574</v>
-      </c>
       <c r="I4" t="s">
         <v>30</v>
       </c>
@@ -4632,14 +4640,6 @@
       <c r="F5">
         <v>2.1463000000000001</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>0.98425925925925928</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1.0159924741298212</v>
-      </c>
       <c r="I5">
         <f>AVERAGE(L:L)</f>
         <v>31.42</v>
@@ -4668,14 +4668,6 @@
       <c r="F6">
         <v>27.655100000000001</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0.98090327633468199</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1.019468508390222</v>
-      </c>
       <c r="P6">
         <v>341</v>
       </c>
@@ -4696,14 +4688,6 @@
       <c r="F7">
         <v>285.39600000000002</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>0.98137662941288306</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1.0189767822352347</v>
-      </c>
       <c r="L7">
         <v>32</v>
       </c>
@@ -4724,14 +4708,6 @@
       <c r="F8">
         <v>161.62299999999999</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0.98379267241902402</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1.0164743324842258</v>
-      </c>
       <c r="P8">
         <v>338</v>
       </c>
@@ -4752,14 +4728,6 @@
       <c r="F9">
         <v>71.982699999999994</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0.99802714707637918</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>1.0019767527660948</v>
-      </c>
       <c r="L9">
         <v>31</v>
       </c>
@@ -4780,14 +4748,6 @@
       <c r="F10">
         <v>195.92699999999999</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0.99854581703623679</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1.0014563006914188</v>
-      </c>
       <c r="I10" t="s">
         <v>29</v>
       </c>
@@ -4796,10 +4756,6 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="G11">
-        <f>AVERAGE(G6:G10)</f>
-        <v>0.98852910845584108</v>
-      </c>
       <c r="I11">
         <f>AVERAGE(P:P)</f>
         <v>340.16</v>
@@ -4851,9 +4807,13 @@
       <c r="C16">
         <v>49.591999999999999</v>
       </c>
-      <c r="D16">
-        <f>B16/B3</f>
-        <v>1.1944444444444446</v>
+      <c r="E16">
+        <f>E3/E3</f>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>B3/E3</f>
+        <v>1.2538787917168006</v>
       </c>
       <c r="P16">
         <v>338</v>
@@ -4869,9 +4829,13 @@
       <c r="C17">
         <v>2.9514900000000002</v>
       </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D23" si="2">B17/B4</f>
-        <v>1.7002192982456141</v>
+      <c r="E17">
+        <f t="shared" ref="E17:E23" si="0">E4/E4</f>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F23" si="1">B4/E4</f>
+        <v>1.0214490516100574</v>
       </c>
       <c r="L17">
         <v>32</v>
@@ -4887,9 +4851,13 @@
       <c r="C18">
         <v>1.35182</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>1.7294072004965859</v>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>1.0159924741298212</v>
       </c>
       <c r="P18">
         <v>338</v>
@@ -4905,9 +4873,13 @@
       <c r="C19">
         <v>334.51400000000001</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>1.7755645477091764</v>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>1.019468508390222</v>
       </c>
       <c r="L19">
         <v>31</v>
@@ -4923,9 +4895,13 @@
       <c r="C20">
         <v>60.207700000000003</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>1.7734984049183444</v>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>1.0189767822352347</v>
       </c>
       <c r="P20">
         <v>338</v>
@@ -4941,9 +4917,13 @@
       <c r="C21">
         <v>121.864</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>1.7672843776167764</v>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1.0164743324842258</v>
       </c>
       <c r="L21">
         <v>32</v>
@@ -4959,9 +4939,13 @@
       <c r="C22">
         <v>77.928200000000004</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>1.8092340369454498</v>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1.0019767527660948</v>
       </c>
       <c r="P22">
         <v>342</v>
@@ -4977,9 +4961,13 @@
       <c r="C23">
         <v>219.64699999999999</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>1.7548942020383422</v>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1.0014563006914188</v>
       </c>
       <c r="L23">
         <v>32</v>

</xml_diff>

<commit_message>
filled benchmarks for mandelbrot and more main text
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28780" windowHeight="16340" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
     <sheet name="dopencl summary" sheetId="2" r:id="rId2"/>
     <sheet name="Aparapi Matrix" sheetId="3" r:id="rId3"/>
-    <sheet name="Sharded Matrix" sheetId="4" r:id="rId4"/>
-    <sheet name="cluster ut" sheetId="5" r:id="rId5"/>
+    <sheet name="cluster ut" sheetId="5" r:id="rId4"/>
+    <sheet name="Sharded Matrix" sheetId="4" r:id="rId5"/>
+    <sheet name="Sharded Mandelbrot" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="40">
   <si>
     <t>Local</t>
   </si>
@@ -126,6 +127,24 @@
   <si>
     <t>Original by hand</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>10 shards</t>
+  </si>
+  <si>
+    <t>2 shards</t>
+  </si>
+  <si>
+    <t>100000 iterations</t>
+  </si>
+  <si>
+    <t>1 Device</t>
+  </si>
 </sst>
 </file>
 
@@ -213,8 +232,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="757">
+  <cellStyleXfs count="761">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -986,7 +1009,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="757">
+  <cellStyles count="761">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1365,6 +1388,8 @@
     <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1743,6 +1768,8 @@
     <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4553,7 +4580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P203"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="G16" sqref="G16:G23"/>
     </sheetView>
   </sheetViews>
@@ -5917,285 +5944,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J1:Q12"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="10:17">
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="10:17">
-      <c r="J3">
-        <v>1000</v>
-      </c>
-      <c r="K3">
-        <v>481.4</v>
-      </c>
-      <c r="L3">
-        <v>6.12</v>
-      </c>
-      <c r="M3">
-        <v>535.20000000000005</v>
-      </c>
-      <c r="N3">
-        <v>10.23</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P9" si="0">K3/M3</f>
-        <v>0.89947683109118071</v>
-      </c>
-      <c r="Q3">
-        <f>M3/K3</f>
-        <v>1.1117573743248859</v>
-      </c>
-    </row>
-    <row r="4" spans="10:17">
-      <c r="J4">
-        <v>2000</v>
-      </c>
-      <c r="K4">
-        <v>2139.1999999999998</v>
-      </c>
-      <c r="L4">
-        <v>15.16</v>
-      </c>
-      <c r="M4">
-        <v>2719.2</v>
-      </c>
-      <c r="N4">
-        <v>31.84</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0.78670197116799057</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q12" si="1">M4/K4</f>
-        <v>1.2711293941660433</v>
-      </c>
-    </row>
-    <row r="5" spans="10:17">
-      <c r="J5">
-        <v>3000</v>
-      </c>
-      <c r="K5">
-        <v>5655</v>
-      </c>
-      <c r="L5">
-        <v>48.73</v>
-      </c>
-      <c r="M5">
-        <v>7796.2</v>
-      </c>
-      <c r="N5">
-        <v>29.48</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0.72535337728637028</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>1.3786383731211318</v>
-      </c>
-    </row>
-    <row r="6" spans="10:17">
-      <c r="J6">
-        <v>4000</v>
-      </c>
-      <c r="K6">
-        <v>11626.4</v>
-      </c>
-      <c r="L6">
-        <v>120.09</v>
-      </c>
-      <c r="M6">
-        <v>16915</v>
-      </c>
-      <c r="N6">
-        <v>40.14</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0.68734259532958908</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>1.4548785522603729</v>
-      </c>
-    </row>
-    <row r="7" spans="10:17">
-      <c r="J7">
-        <v>5000</v>
-      </c>
-      <c r="K7">
-        <v>20279.8</v>
-      </c>
-      <c r="L7">
-        <v>33.65</v>
-      </c>
-      <c r="M7">
-        <v>31284.799999999999</v>
-      </c>
-      <c r="N7">
-        <v>64.569999999999993</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.64823172914642258</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>1.5426582116194441</v>
-      </c>
-    </row>
-    <row r="8" spans="10:17">
-      <c r="J8">
-        <v>6000</v>
-      </c>
-      <c r="K8">
-        <v>32804.6</v>
-      </c>
-      <c r="L8">
-        <v>232.71</v>
-      </c>
-      <c r="M8">
-        <v>52027.4</v>
-      </c>
-      <c r="N8">
-        <v>109.6</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0.63052545389544734</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>1.5859787956567069</v>
-      </c>
-    </row>
-    <row r="9" spans="10:17">
-      <c r="J9">
-        <v>7000</v>
-      </c>
-      <c r="K9">
-        <v>49707.8</v>
-      </c>
-      <c r="L9">
-        <v>421.68</v>
-      </c>
-      <c r="M9">
-        <v>81267.399999999994</v>
-      </c>
-      <c r="N9">
-        <v>349.61</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0.6116573189249318</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>1.6349023694470484</v>
-      </c>
-    </row>
-    <row r="10" spans="10:17">
-      <c r="J10">
-        <v>8000</v>
-      </c>
-      <c r="K10">
-        <v>70965.399999999994</v>
-      </c>
-      <c r="L10">
-        <v>437.87</v>
-      </c>
-      <c r="M10">
-        <v>118798</v>
-      </c>
-      <c r="N10">
-        <v>311.64</v>
-      </c>
-      <c r="P10">
-        <f>K10/M10</f>
-        <v>0.5973619084496371</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>1.6740270610748338</v>
-      </c>
-    </row>
-    <row r="11" spans="10:17">
-      <c r="J11">
-        <v>9000</v>
-      </c>
-      <c r="K11">
-        <v>98685.6</v>
-      </c>
-      <c r="L11">
-        <v>116.37</v>
-      </c>
-      <c r="M11">
-        <v>168573.4</v>
-      </c>
-      <c r="N11">
-        <v>243.48</v>
-      </c>
-      <c r="P11">
-        <f t="shared" ref="P11:P12" si="2">K11/M11</f>
-        <v>0.58541620445455811</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>1.708186402068792</v>
-      </c>
-    </row>
-    <row r="12" spans="10:17">
-      <c r="J12">
-        <v>10000</v>
-      </c>
-      <c r="K12">
-        <v>131682.6</v>
-      </c>
-      <c r="L12">
-        <v>602.36</v>
-      </c>
-      <c r="M12">
-        <v>228206.6</v>
-      </c>
-      <c r="N12">
-        <v>1147.06</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="2"/>
-        <v>0.57703239082480529</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>1.7330049680064032</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N45"/>
   <sheetViews>
@@ -7532,4 +7280,530 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="J1:Q12"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="10:17">
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="10:17">
+      <c r="J3">
+        <v>1000</v>
+      </c>
+      <c r="K3">
+        <v>481.4</v>
+      </c>
+      <c r="L3">
+        <v>6.12</v>
+      </c>
+      <c r="M3">
+        <v>535.20000000000005</v>
+      </c>
+      <c r="N3">
+        <v>10.23</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="0">K3/M3</f>
+        <v>0.89947683109118071</v>
+      </c>
+      <c r="Q3">
+        <f>M3/K3</f>
+        <v>1.1117573743248859</v>
+      </c>
+    </row>
+    <row r="4" spans="10:17">
+      <c r="J4">
+        <v>2000</v>
+      </c>
+      <c r="K4">
+        <v>2139.1999999999998</v>
+      </c>
+      <c r="L4">
+        <v>15.16</v>
+      </c>
+      <c r="M4">
+        <v>2719.2</v>
+      </c>
+      <c r="N4">
+        <v>31.84</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.78670197116799057</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q12" si="1">M4/K4</f>
+        <v>1.2711293941660433</v>
+      </c>
+    </row>
+    <row r="5" spans="10:17">
+      <c r="J5">
+        <v>3000</v>
+      </c>
+      <c r="K5">
+        <v>5655</v>
+      </c>
+      <c r="L5">
+        <v>48.73</v>
+      </c>
+      <c r="M5">
+        <v>7796.2</v>
+      </c>
+      <c r="N5">
+        <v>29.48</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.72535337728637028</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>1.3786383731211318</v>
+      </c>
+    </row>
+    <row r="6" spans="10:17">
+      <c r="J6">
+        <v>4000</v>
+      </c>
+      <c r="K6">
+        <v>11626.4</v>
+      </c>
+      <c r="L6">
+        <v>120.09</v>
+      </c>
+      <c r="M6">
+        <v>16915</v>
+      </c>
+      <c r="N6">
+        <v>40.14</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.68734259532958908</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>1.4548785522603729</v>
+      </c>
+    </row>
+    <row r="7" spans="10:17">
+      <c r="J7">
+        <v>5000</v>
+      </c>
+      <c r="K7">
+        <v>20279.8</v>
+      </c>
+      <c r="L7">
+        <v>33.65</v>
+      </c>
+      <c r="M7">
+        <v>31284.799999999999</v>
+      </c>
+      <c r="N7">
+        <v>64.569999999999993</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.64823172914642258</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>1.5426582116194441</v>
+      </c>
+    </row>
+    <row r="8" spans="10:17">
+      <c r="J8">
+        <v>6000</v>
+      </c>
+      <c r="K8">
+        <v>32804.6</v>
+      </c>
+      <c r="L8">
+        <v>232.71</v>
+      </c>
+      <c r="M8">
+        <v>52027.4</v>
+      </c>
+      <c r="N8">
+        <v>109.6</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0.63052545389544734</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>1.5859787956567069</v>
+      </c>
+    </row>
+    <row r="9" spans="10:17">
+      <c r="J9">
+        <v>7000</v>
+      </c>
+      <c r="K9">
+        <v>49707.8</v>
+      </c>
+      <c r="L9">
+        <v>421.68</v>
+      </c>
+      <c r="M9">
+        <v>81267.399999999994</v>
+      </c>
+      <c r="N9">
+        <v>349.61</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.6116573189249318</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>1.6349023694470484</v>
+      </c>
+    </row>
+    <row r="10" spans="10:17">
+      <c r="J10">
+        <v>8000</v>
+      </c>
+      <c r="K10">
+        <v>70965.399999999994</v>
+      </c>
+      <c r="L10">
+        <v>437.87</v>
+      </c>
+      <c r="M10">
+        <v>118798</v>
+      </c>
+      <c r="N10">
+        <v>311.64</v>
+      </c>
+      <c r="P10">
+        <f>K10/M10</f>
+        <v>0.5973619084496371</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>1.6740270610748338</v>
+      </c>
+    </row>
+    <row r="11" spans="10:17">
+      <c r="J11">
+        <v>9000</v>
+      </c>
+      <c r="K11">
+        <v>98685.6</v>
+      </c>
+      <c r="L11">
+        <v>116.37</v>
+      </c>
+      <c r="M11">
+        <v>168573.4</v>
+      </c>
+      <c r="N11">
+        <v>243.48</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P12" si="2">K11/M11</f>
+        <v>0.58541620445455811</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>1.708186402068792</v>
+      </c>
+    </row>
+    <row r="12" spans="10:17">
+      <c r="J12">
+        <v>10000</v>
+      </c>
+      <c r="K12">
+        <v>131682.6</v>
+      </c>
+      <c r="L12">
+        <v>602.36</v>
+      </c>
+      <c r="M12">
+        <v>228206.6</v>
+      </c>
+      <c r="N12">
+        <v>1147.06</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>0.57703239082480529</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>1.7330049680064032</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3000</v>
+      </c>
+      <c r="B4">
+        <v>7561.8</v>
+      </c>
+      <c r="C4">
+        <v>31.84</v>
+      </c>
+      <c r="E4">
+        <v>13659</v>
+      </c>
+      <c r="F4">
+        <v>407.35</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>E4/B4</f>
+        <v>1.8063159565182894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4000</v>
+      </c>
+      <c r="B5">
+        <v>13699.2</v>
+      </c>
+      <c r="C5">
+        <v>914.66</v>
+      </c>
+      <c r="E5">
+        <v>24844.400000000001</v>
+      </c>
+      <c r="F5">
+        <v>925.68</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I11" si="0">E5/B5</f>
+        <v>1.8135657556645643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5000</v>
+      </c>
+      <c r="B6">
+        <v>20991.8</v>
+      </c>
+      <c r="C6">
+        <v>510.17</v>
+      </c>
+      <c r="E6">
+        <v>39092.199999999997</v>
+      </c>
+      <c r="F6">
+        <v>1001.62</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.8622605017197191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6000</v>
+      </c>
+      <c r="B7">
+        <v>30064.6</v>
+      </c>
+      <c r="C7">
+        <v>774.91</v>
+      </c>
+      <c r="E7">
+        <v>56131.199999999997</v>
+      </c>
+      <c r="F7">
+        <v>1591.17</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.8670196842798508</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7000</v>
+      </c>
+      <c r="B8">
+        <v>40989.199999999997</v>
+      </c>
+      <c r="C8">
+        <v>1026.77</v>
+      </c>
+      <c r="E8">
+        <v>76742.399999999994</v>
+      </c>
+      <c r="F8">
+        <v>1193.58</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.8722590340870278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8000</v>
+      </c>
+      <c r="B9">
+        <v>53303</v>
+      </c>
+      <c r="C9">
+        <v>1001.87</v>
+      </c>
+      <c r="E9">
+        <v>100000.6</v>
+      </c>
+      <c r="F9">
+        <v>1337.9</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>1.8760782695157872</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9000</v>
+      </c>
+      <c r="B10">
+        <v>67699.199999999997</v>
+      </c>
+      <c r="C10">
+        <v>719.62</v>
+      </c>
+      <c r="E10">
+        <v>126908.2</v>
+      </c>
+      <c r="F10">
+        <v>1108.58</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>1.8745893599924373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10000</v>
+      </c>
+      <c r="B11">
+        <v>83704.2</v>
+      </c>
+      <c r="C11">
+        <v>1197.97</v>
+      </c>
+      <c r="E11">
+        <v>156677</v>
+      </c>
+      <c r="F11">
+        <v>1194.72</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.8717937690103963</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added benchmarking setup graphs
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="26520" windowHeight="16140" tabRatio="500" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="26520" windowHeight="16200" tabRatio="500" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="66">
   <si>
     <t>Local</t>
   </si>
@@ -214,6 +214,18 @@
   <si>
     <t>1 device with 144 cores connected via 1 gbit</t>
   </si>
+  <si>
+    <t>Matrix 1</t>
+  </si>
+  <si>
+    <t>Matrix 2</t>
+  </si>
+  <si>
+    <t>Mandelbrot 1</t>
+  </si>
+  <si>
+    <t>Mandelbrot 2</t>
+  </si>
 </sst>
 </file>
 
@@ -301,8 +313,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1001">
+  <cellStyleXfs count="1021">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1318,7 +1350,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1001">
+  <cellStyles count="1021">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1819,6 +1851,16 @@
     <cellStyle name="Followed Hyperlink" xfId="996" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="998" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1020" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2319,6 +2361,16 @@
     <cellStyle name="Hyperlink" xfId="995" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="997" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1013" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1015" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1017" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1019" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8423,10 +8475,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8923,6 +8975,78 @@
       <c r="N17">
         <f>AVERAGE(C17,E17,G17,I17,K17)</f>
         <v>29.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24">
+        <v>307200000</v>
+      </c>
+      <c r="C24">
+        <f>B24/1024/1024</f>
+        <v>292.96875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25">
+        <v>172800000</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C29" si="0">B25/1024/1024</f>
+        <v>164.794921875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26">
+        <v>1600000</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>1.52587890625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27">
+        <v>6400000</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>6.103515625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28">
+        <v>120003200</v>
+      </c>
+      <c r="C28">
+        <f>B28/1000/1000</f>
+        <v>120.00319999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>4608000</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>4.39453125</v>
       </c>
     </row>
   </sheetData>
@@ -8941,7 +9065,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
wrote some more evaluation for local clusters
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="26520" windowHeight="16200" tabRatio="500" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="28560" windowHeight="16240" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
   <si>
     <t>Local</t>
   </si>
@@ -149,10 +149,16 @@
     <t>1 Device</t>
   </si>
   <si>
+    <t>___________________</t>
+  </si>
+  <si>
     <t>Matrix Big</t>
   </si>
   <si>
     <t>Matrix Small</t>
+  </si>
+  <si>
+    <t>Matrix</t>
   </si>
   <si>
     <t>Mandelbrot Big</t>
@@ -189,9 +195,6 @@
   </si>
   <si>
     <t>Run 5</t>
-  </si>
-  <si>
-    <t>Subtract 2 seconds</t>
   </si>
   <si>
     <t>1 local device 8 cores no dopencl</t>
@@ -313,8 +316,136 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1021">
+  <cellStyleXfs count="1149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1350,7 +1481,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1021">
+  <cellStyles count="1149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1861,6 +1992,70 @@
     <cellStyle name="Followed Hyperlink" xfId="1016" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1018" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1032" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1034" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1036" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1038" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1040" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1042" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1044" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1046" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1048" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1050" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1052" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1054" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1056" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1058" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1060" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1062" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1064" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1066" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1068" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1070" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1072" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1074" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1076" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1078" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1080" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1082" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1084" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1086" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1088" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1090" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1092" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1094" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1096" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1098" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2371,6 +2566,70 @@
     <cellStyle name="Hyperlink" xfId="1015" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1017" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1019" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1021" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1025" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1027" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1029" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1031" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1033" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1035" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1037" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1039" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1041" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1043" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1045" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1047" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1049" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1051" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1053" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1055" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1057" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1059" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1061" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1063" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1065" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1067" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1069" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1071" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1073" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1075" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1077" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1079" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1081" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1083" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1085" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1087" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1089" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1091" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1093" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1095" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1097" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1099" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6613,7 +6872,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7952,7 +8211,7 @@
   <dimension ref="J1:Q12"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8234,15 +8493,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -8256,7 +8515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -8270,7 +8529,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3000</v>
       </c>
@@ -8294,7 +8553,7 @@
         <v>1.8063159565182894</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4000</v>
       </c>
@@ -8318,7 +8577,7 @@
         <v>1.8135657556645643</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -8342,7 +8601,7 @@
         <v>1.8622605017197191</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6000</v>
       </c>
@@ -8366,7 +8625,7 @@
         <v>1.8670196842798508</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7000</v>
       </c>
@@ -8390,7 +8649,7 @@
         <v>1.8722590340870278</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8000</v>
       </c>
@@ -8414,7 +8673,7 @@
         <v>1.8760782695157872</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -8438,7 +8697,7 @@
         <v>1.8745893599924373</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10000</v>
       </c>
@@ -8460,6 +8719,16 @@
       <c r="I11">
         <f t="shared" si="0"/>
         <v>1.8717937690103963</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="I12">
+        <f>MAX(I4:I11)</f>
+        <v>1.8760782695157872</v>
+      </c>
+      <c r="J12">
+        <f>MIN(I4:I11)</f>
+        <v>1.8063159565182894</v>
       </c>
     </row>
   </sheetData>
@@ -8475,10 +8744,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8489,16 +8758,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
       </c>
       <c r="F1">
         <v>1</v>
@@ -8518,120 +8784,120 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2">
-        <v>219727</v>
+        <v>219360</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2">
-        <v>106274</v>
+        <v>170788</v>
       </c>
       <c r="G2">
-        <v>112798</v>
+        <v>177283</v>
       </c>
       <c r="H2">
-        <v>112170</v>
+        <v>173015</v>
       </c>
       <c r="I2">
-        <v>167087</v>
+        <v>123402</v>
       </c>
       <c r="J2">
-        <v>174579</v>
+        <v>188585</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="B3">
-        <v>218111</v>
+        <v>218884</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3">
-        <v>51620</v>
+        <v>127980</v>
       </c>
       <c r="G3">
-        <v>105284</v>
+        <v>205371</v>
       </c>
       <c r="H3">
-        <v>104010</v>
+        <v>101222</v>
       </c>
       <c r="I3">
-        <v>73347</v>
+        <v>158770</v>
       </c>
       <c r="J3">
-        <v>172979</v>
+        <v>106361</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="B4">
-        <v>217747</v>
+        <v>218809</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F4">
-        <v>90452</v>
+        <v>139795</v>
       </c>
       <c r="G4">
-        <v>118608</v>
+        <v>197183</v>
       </c>
       <c r="H4">
-        <v>96995</v>
+        <v>26700</v>
       </c>
       <c r="I4">
-        <v>99810</v>
+        <v>30764</v>
       </c>
       <c r="J4">
-        <v>165424</v>
+        <v>189663</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="B5">
-        <v>218530</v>
+        <v>219336</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <v>41684</v>
+        <v>70767</v>
       </c>
       <c r="G5">
-        <v>96312</v>
+        <v>188219</v>
       </c>
       <c r="H5">
-        <v>75213</v>
+        <v>174485</v>
       </c>
       <c r="I5">
-        <v>145171</v>
+        <v>60559</v>
       </c>
       <c r="J5">
-        <v>105717</v>
+        <v>170221</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="B6">
-        <v>218978</v>
+        <v>219688</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F6">
-        <v>177100</v>
+        <v>190238</v>
       </c>
       <c r="G6">
-        <v>187509</v>
+        <v>205343</v>
       </c>
       <c r="H6">
-        <v>111649</v>
+        <v>180203</v>
       </c>
       <c r="I6">
-        <v>156231</v>
+        <v>171166</v>
       </c>
       <c r="J6">
-        <v>9152</v>
+        <v>215037</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8642,78 +8908,78 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7">
-        <v>161706</v>
+        <v>162523</v>
       </c>
       <c r="G7">
-        <v>144413</v>
+        <v>13006</v>
       </c>
       <c r="H7">
-        <v>125044</v>
+        <v>206069</v>
       </c>
       <c r="I7">
-        <v>181909</v>
+        <v>129823</v>
       </c>
       <c r="J7">
-        <v>214364</v>
+        <v>12414</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="B8">
         <f>AVERAGE(B2:B6)</f>
-        <v>218618.6</v>
+        <v>219215.4</v>
       </c>
       <c r="C8">
         <f>STDEV(B2:B6)</f>
-        <v>771.8343734247652</v>
+        <v>365.30507798277318</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
         <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
         <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
         <v>35</v>
@@ -8721,265 +8987,265 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12">
-        <v>20821</v>
+        <v>20629</v>
       </c>
       <c r="C12">
-        <v>103</v>
+        <v>448</v>
       </c>
       <c r="D12">
-        <v>20717</v>
+        <v>20521</v>
       </c>
       <c r="E12">
-        <v>105</v>
+        <v>383</v>
       </c>
       <c r="F12">
-        <v>20714</v>
+        <v>20625</v>
       </c>
       <c r="G12">
-        <v>91</v>
+        <v>325</v>
       </c>
       <c r="H12">
-        <v>20593</v>
+        <v>20584</v>
       </c>
       <c r="I12">
-        <v>284</v>
+        <v>433</v>
       </c>
       <c r="J12">
-        <v>20585</v>
+        <v>20676</v>
       </c>
       <c r="K12">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="M12">
         <f>AVERAGE(B12,D12,F12,H12,J12)</f>
-        <v>20686</v>
+        <v>20607</v>
       </c>
       <c r="N12">
         <f>AVERAGE(C12,E12,G12,I12,K12)</f>
-        <v>165.6</v>
+        <v>387.2</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13">
-        <v>8496</v>
+        <v>8693</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="D13">
-        <v>8616</v>
+        <v>8605</v>
       </c>
       <c r="E13">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="F13">
-        <v>8654</v>
+        <v>8548</v>
       </c>
       <c r="G13">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="H13">
-        <v>8683</v>
+        <v>8642</v>
       </c>
       <c r="I13">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="J13">
-        <v>8696</v>
+        <v>8537</v>
       </c>
       <c r="K13">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M13">
         <f>AVERAGE(B13,D13,F13,H13,J13)</f>
-        <v>8629</v>
+        <v>8605</v>
       </c>
       <c r="N13">
         <f>AVERAGE(C13,E13,G13,I13,K13)</f>
-        <v>87.6</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14">
-        <v>3376</v>
+        <v>3312</v>
       </c>
       <c r="C14">
-        <v>4260</v>
+        <v>4144</v>
       </c>
       <c r="D14">
-        <v>3241</v>
+        <v>3393</v>
       </c>
       <c r="E14">
-        <v>4026</v>
+        <v>4275</v>
       </c>
       <c r="F14">
-        <v>3383</v>
+        <v>3448</v>
       </c>
       <c r="G14">
-        <v>4291</v>
+        <v>4294</v>
       </c>
       <c r="H14">
-        <v>3361</v>
+        <v>3443</v>
       </c>
       <c r="I14">
-        <v>4248</v>
+        <v>4292</v>
       </c>
       <c r="J14">
-        <v>3458</v>
+        <v>3476</v>
       </c>
       <c r="K14">
-        <v>4309</v>
+        <v>4337</v>
       </c>
       <c r="M14">
         <f>AVERAGE(B14,D14,F14,H14,J14)</f>
-        <v>3363.8</v>
+        <v>3414.4</v>
       </c>
       <c r="N14">
         <f>AVERAGE(C14,E14,G14,I14,K14)</f>
-        <v>4226.8</v>
+        <v>4268.3999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15">
-        <v>8151</v>
+        <v>8141</v>
       </c>
       <c r="C15">
-        <v>10329</v>
+        <v>10285</v>
       </c>
       <c r="D15">
-        <v>7961</v>
+        <v>8139</v>
       </c>
       <c r="E15">
-        <v>10224</v>
+        <v>10313</v>
       </c>
       <c r="F15">
-        <v>7685</v>
+        <v>8059</v>
       </c>
       <c r="G15">
-        <v>9779</v>
+        <v>10301</v>
       </c>
       <c r="H15">
-        <v>7974</v>
+        <v>8106</v>
       </c>
       <c r="I15">
-        <v>10236</v>
+        <v>10289</v>
       </c>
       <c r="J15">
-        <v>7882</v>
+        <v>8170</v>
       </c>
       <c r="K15">
-        <v>10080</v>
+        <v>10340</v>
       </c>
       <c r="M15">
         <f>AVERAGE(B15,D15,F15,H15,J15)</f>
-        <v>7930.6</v>
+        <v>8123</v>
       </c>
       <c r="N15">
         <f>AVERAGE(C15,E15,G15,I15,K15)</f>
-        <v>10129.6</v>
+        <v>10305.6</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16">
-        <v>932</v>
+        <v>938</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>602</v>
       </c>
       <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>932</v>
+      </c>
+      <c r="G16">
+        <v>26</v>
+      </c>
+      <c r="H16">
+        <v>602</v>
+      </c>
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>602</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>601</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
       <c r="J16">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M16">
         <f>AVERAGE(B16,D16,F16,H16,J16)</f>
-        <v>667.8</v>
+        <v>735.4</v>
       </c>
       <c r="N16">
         <f>AVERAGE(C16,E16,G16,I16,K16)</f>
-        <v>5.2</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>936</v>
       </c>
       <c r="E17">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F17">
-        <v>948</v>
+        <v>603</v>
       </c>
       <c r="G17">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="H17">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="I17">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J17">
-        <v>941</v>
+        <v>928</v>
       </c>
       <c r="K17">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="M17">
         <f>AVERAGE(B17,D17,F17,H17,J17)</f>
-        <v>874.8</v>
+        <v>801.2</v>
       </c>
       <c r="N17">
         <f>AVERAGE(C17,E17,G17,I17,K17)</f>
-        <v>29.4</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24">
         <v>307200000</v>
@@ -8991,7 +9257,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25">
         <v>172800000</v>
@@ -9003,7 +9269,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B26">
         <v>1600000</v>
@@ -9015,7 +9281,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27">
         <v>6400000</v>
@@ -9027,7 +9293,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28">
         <v>120003200</v>
@@ -9039,7 +9305,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29">
         <v>4608000</v>
@@ -9047,6 +9313,19 @@
       <c r="C29">
         <f t="shared" si="0"/>
         <v>4.39453125</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6">
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="5:6">
+      <c r="E59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59">
+        <v>358400000</v>
       </c>
     </row>
   </sheetData>
@@ -9062,10 +9341,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9076,379 +9355,146 @@
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>2</v>
-      </c>
-      <c r="H1">
-        <v>3</v>
-      </c>
-      <c r="I1">
-        <v>4</v>
-      </c>
-      <c r="J1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2">
-        <v>116228</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2">
-        <v>102519</v>
-      </c>
-      <c r="G2">
-        <v>91654</v>
-      </c>
-      <c r="H2">
-        <v>98568</v>
-      </c>
-      <c r="I2">
-        <v>71264</v>
-      </c>
-      <c r="J2">
-        <v>67014</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>127923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3">
-        <v>120633</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3">
-        <v>85990</v>
-      </c>
-      <c r="G3">
-        <v>47014</v>
-      </c>
-      <c r="H3">
-        <v>106617</v>
-      </c>
-      <c r="I3">
-        <v>97826</v>
-      </c>
-      <c r="J3">
-        <v>63937</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>121524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="B4">
-        <v>115257</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4">
-        <v>79771</v>
-      </c>
-      <c r="G4">
-        <v>48511</v>
-      </c>
-      <c r="H4">
-        <v>83386</v>
-      </c>
-      <c r="I4">
-        <v>58594</v>
-      </c>
-      <c r="J4">
-        <v>42437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5">
-        <v>130666</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5">
-        <v>80996</v>
-      </c>
-      <c r="G5">
-        <v>83334</v>
-      </c>
-      <c r="H5">
-        <v>99836</v>
-      </c>
-      <c r="I5">
-        <v>119560</v>
-      </c>
-      <c r="J5">
-        <v>53442</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6">
-        <v>126599</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6">
-        <v>112194</v>
-      </c>
-      <c r="G6">
-        <v>89440</v>
-      </c>
-      <c r="H6">
-        <v>111832</v>
-      </c>
-      <c r="I6">
-        <v>99558</v>
-      </c>
-      <c r="J6">
-        <v>77932</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>123627</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7">
-        <v>36430</v>
-      </c>
-      <c r="G7">
-        <v>92526</v>
-      </c>
-      <c r="H7">
-        <v>114394</v>
-      </c>
-      <c r="I7">
-        <v>130640</v>
-      </c>
-      <c r="J7">
-        <v>74926</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:3">
       <c r="B8">
         <f>AVERAGE(B2:B6)</f>
-        <v>121876.6</v>
+        <v>124358</v>
       </c>
       <c r="C8">
         <f>STDEV(B2:B6)</f>
-        <v>6648.8145785545858</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>3261.5289359439998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>59</v>
       </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
       <c r="B13">
-        <v>67417</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13">
-        <v>64133</v>
-      </c>
-      <c r="G13">
-        <v>54266</v>
-      </c>
-      <c r="H13">
-        <v>75562</v>
-      </c>
-      <c r="I13">
-        <v>60219</v>
-      </c>
-      <c r="J13">
-        <v>46762</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>67691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <v>56733</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14">
-        <v>42422</v>
-      </c>
-      <c r="G14">
-        <v>19314</v>
-      </c>
-      <c r="H14">
-        <v>18021</v>
-      </c>
-      <c r="I14">
-        <v>66412</v>
-      </c>
-      <c r="J14">
-        <v>37184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>66210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15">
-        <v>75593</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15">
-        <v>24295</v>
-      </c>
-      <c r="G15">
-        <v>32703</v>
-      </c>
-      <c r="H15">
-        <v>53555</v>
-      </c>
-      <c r="I15">
-        <v>27518</v>
-      </c>
-      <c r="J15">
-        <v>38616</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>62268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="B16">
-        <v>69173</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16">
-        <v>32815</v>
-      </c>
-      <c r="G16">
-        <v>30643</v>
-      </c>
-      <c r="H16">
-        <v>40023</v>
-      </c>
-      <c r="I16">
-        <v>38672</v>
-      </c>
-      <c r="J16">
-        <v>36419</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+        <v>57949</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17">
-        <v>52885</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17">
-        <v>67340</v>
-      </c>
-      <c r="G17">
-        <v>47910</v>
-      </c>
-      <c r="H17">
-        <v>69856</v>
-      </c>
-      <c r="I17">
-        <v>66848</v>
-      </c>
-      <c r="J17">
-        <v>52684</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+        <v>54772</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18">
-        <v>56454</v>
-      </c>
-      <c r="G18">
-        <v>46157</v>
-      </c>
-      <c r="H18">
-        <v>54538</v>
-      </c>
-      <c r="I18">
-        <v>51029</v>
-      </c>
-      <c r="J18">
-        <v>52827</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19">
         <f>AVERAGE(B13:B17)</f>
-        <v>64360.2</v>
+        <v>61778</v>
       </c>
       <c r="C19">
         <f>STDEV(B13:B17)</f>
-        <v>9334.5763267541934</v>
+        <v>5444.9878328606028</v>
+      </c>
+      <c r="F19">
+        <v>219215.4</v>
+      </c>
+      <c r="G19">
+        <v>124358</v>
+      </c>
+      <c r="H19">
+        <v>61778</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f>G19/F19</f>
+        <v>0.56728678733337168</v>
+      </c>
+      <c r="H20">
+        <f>H19/F19</f>
+        <v>0.28181414261954224</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f>F20/G20</f>
+        <v>1.7627768217565416</v>
+      </c>
+      <c r="H21">
+        <f>F20/H20</f>
+        <v>3.5484379552591538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ec2 hybrid cluster network performance
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="28560" windowHeight="16240" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="28560" windowHeight="16240" tabRatio="500" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Full Benchmark Single Device" sheetId="9" r:id="rId7"/>
     <sheet name="Full Benchmark local" sheetId="7" r:id="rId8"/>
     <sheet name="Full Benchmark Hybrid" sheetId="8" r:id="rId9"/>
+    <sheet name="EC2 Hybrid Network Measurement" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="71">
   <si>
     <t>Local</t>
   </si>
@@ -229,6 +230,18 @@
   <si>
     <t>Mandelbrot 2</t>
   </si>
+  <si>
+    <t>t2.micro</t>
+  </si>
+  <si>
+    <t>r4.8xlarge</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
 </sst>
 </file>
 
@@ -316,8 +329,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1149">
+  <cellStyleXfs count="1163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1481,7 +1508,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1149">
+  <cellStyles count="1163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2056,6 +2083,13 @@
     <cellStyle name="Followed Hyperlink" xfId="1144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2630,6 +2664,13 @@
     <cellStyle name="Hyperlink" xfId="1143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4367,6 +4408,567 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="3:6">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6">
+      <c r="C2">
+        <v>175</v>
+      </c>
+      <c r="F2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>189</v>
+      </c>
+      <c r="F3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4">
+        <v>199</v>
+      </c>
+      <c r="F4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="C5">
+        <v>168</v>
+      </c>
+      <c r="F5">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6">
+        <v>178</v>
+      </c>
+      <c r="F6">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7">
+        <v>178</v>
+      </c>
+      <c r="F7">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="C8">
+        <v>178</v>
+      </c>
+      <c r="F8">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9">
+        <v>189</v>
+      </c>
+      <c r="F9">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10">
+        <v>199</v>
+      </c>
+      <c r="F10">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11">
+        <v>199</v>
+      </c>
+      <c r="F11">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="C12">
+        <v>199</v>
+      </c>
+      <c r="F12">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="C13">
+        <v>178</v>
+      </c>
+      <c r="F13">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14">
+        <v>178</v>
+      </c>
+      <c r="F14">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="C15">
+        <v>199</v>
+      </c>
+      <c r="F15">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16">
+        <v>199</v>
+      </c>
+      <c r="F16">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17">
+        <v>178</v>
+      </c>
+      <c r="F17">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18">
+        <v>168</v>
+      </c>
+      <c r="F18">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19">
+        <v>178</v>
+      </c>
+      <c r="F19">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20">
+        <v>178</v>
+      </c>
+      <c r="F20">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21">
+        <v>189</v>
+      </c>
+      <c r="F21">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>189</v>
+      </c>
+      <c r="F22">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23">
+        <v>189</v>
+      </c>
+      <c r="F23">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24">
+        <v>199</v>
+      </c>
+      <c r="F24">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25">
+        <v>178</v>
+      </c>
+      <c r="F25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26">
+        <v>178</v>
+      </c>
+      <c r="F26">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27">
+        <v>189</v>
+      </c>
+      <c r="F27">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28">
+        <v>168</v>
+      </c>
+      <c r="F28">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29">
+        <v>168</v>
+      </c>
+      <c r="F29">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30">
+        <v>168</v>
+      </c>
+      <c r="F30">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31">
+        <v>168</v>
+      </c>
+      <c r="F31">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32">
+        <v>178</v>
+      </c>
+      <c r="F32">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33">
+        <v>189</v>
+      </c>
+      <c r="F33">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34">
+        <v>168</v>
+      </c>
+      <c r="F34">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35">
+        <v>157</v>
+      </c>
+      <c r="F35">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="C36">
+        <v>178</v>
+      </c>
+      <c r="F36">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6">
+      <c r="C37">
+        <v>168</v>
+      </c>
+      <c r="F37">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38">
+        <v>168</v>
+      </c>
+      <c r="F38">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6">
+      <c r="C39">
+        <v>189</v>
+      </c>
+      <c r="F39">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40">
+        <v>178</v>
+      </c>
+      <c r="F40">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41">
+        <v>189</v>
+      </c>
+      <c r="F41">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6">
+      <c r="C42">
+        <v>178</v>
+      </c>
+      <c r="F42">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43">
+        <v>199</v>
+      </c>
+      <c r="F43">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44">
+        <v>199</v>
+      </c>
+      <c r="F44">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45">
+        <v>168</v>
+      </c>
+      <c r="F45">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6">
+      <c r="C46">
+        <v>168</v>
+      </c>
+      <c r="F46">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6">
+      <c r="C47">
+        <v>157</v>
+      </c>
+      <c r="F47">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6">
+      <c r="C48">
+        <v>157</v>
+      </c>
+      <c r="F48">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="C49">
+        <v>147</v>
+      </c>
+      <c r="F49">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="C50">
+        <v>157</v>
+      </c>
+      <c r="F50">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="C51">
+        <v>168</v>
+      </c>
+      <c r="F51">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="C52">
+        <v>168</v>
+      </c>
+      <c r="F52">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="C53">
+        <v>189</v>
+      </c>
+      <c r="F53">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="C54">
+        <v>178</v>
+      </c>
+      <c r="F54">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="C55">
+        <v>199</v>
+      </c>
+      <c r="F55">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="C56">
+        <v>189</v>
+      </c>
+      <c r="F56">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="C57">
+        <v>168</v>
+      </c>
+      <c r="F57">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="C58">
+        <v>178</v>
+      </c>
+      <c r="F58">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="C59">
+        <v>178</v>
+      </c>
+      <c r="F59">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="C60">
+        <v>199</v>
+      </c>
+      <c r="F60">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="C61">
+        <v>189</v>
+      </c>
+      <c r="F61">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63">
+        <f>AVERAGE(C2:C61)</f>
+        <v>179.75</v>
+      </c>
+      <c r="F63">
+        <f t="shared" ref="D63:F63" si="0">AVERAGE(F2:F61)</f>
+        <v>456.06666666666666</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64">
+        <f>STDEV(C2:C61)</f>
+        <v>13.182712099757195</v>
+      </c>
+      <c r="F64">
+        <f t="shared" ref="D64:F64" si="1">STDEV(F2:F61)</f>
+        <v>117.94466767416129</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65">
+        <f>MIN(C2:C61)</f>
+        <v>147</v>
+      </c>
+      <c r="F65">
+        <f t="shared" ref="D65:F65" si="2">MIN(F2:F61)</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66">
+        <f>MAX(C2:C61)</f>
+        <v>199</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="D66:F66" si="3">MAX(F2:F61)</f>
+        <v>598</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S46"/>
@@ -8746,7 +9348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
future work and slowly starting to rework older chapters
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28460" windowHeight="17860" tabRatio="500" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28460" windowHeight="16320" tabRatio="500" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dopencl matrix" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2539">
+  <cellStyleXfs count="2555">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2999,7 +3015,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2539">
+  <cellStyles count="2555">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4269,6 +4285,14 @@
     <cellStyle name="Followed Hyperlink" xfId="2534" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2536" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2554" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5538,6 +5562,14 @@
     <cellStyle name="Hyperlink" xfId="2533" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2535" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2553" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9947,8 +9979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56:I58"/>
+    <sheetView showRuler="0" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10692,6 +10724,12 @@
         <v>2.1654189269965154</v>
       </c>
     </row>
+    <row r="38" spans="1:16">
+      <c r="E38" s="1">
+        <f>AVERAGE(E30:E36)</f>
+        <v>2.8505698434313897</v>
+      </c>
+    </row>
     <row r="42" spans="1:16">
       <c r="A42" s="1" t="s">
         <v>107</v>
@@ -10993,6 +11031,12 @@
       <c r="P50" s="1">
         <f>M11/M50</f>
         <v>2.2751760880487644</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="E51" s="1">
+        <f>AVERAGE(E43:E49)</f>
+        <v>3.7349859250104229</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -17378,10 +17422,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17393,7 +17437,7 @@
       </c>
       <c r="E1">
         <f t="shared" ref="C1:E1" si="0">AVERAGE(D:D)</f>
-        <v>9.252711864406777</v>
+        <v>9.4444999999999961</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -17403,7 +17447,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="C2:E2" si="1">STDEV(D:D)</f>
-        <v>2.6052368247275162E-2</v>
+        <v>6.8381407920227455E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -17411,7 +17455,7 @@
         <v>996</v>
       </c>
       <c r="D3">
-        <v>9.26</v>
+        <v>9.3699999999999992</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -17419,7 +17463,7 @@
         <v>986</v>
       </c>
       <c r="D4">
-        <v>9.2799999999999994</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -17427,7 +17471,7 @@
         <v>996</v>
       </c>
       <c r="D5">
-        <v>9.24</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -17435,7 +17479,7 @@
         <v>996</v>
       </c>
       <c r="D6">
-        <v>9.18</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -17443,7 +17487,7 @@
         <v>986</v>
       </c>
       <c r="D7">
-        <v>9.25</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -17451,7 +17495,7 @@
         <v>996</v>
       </c>
       <c r="D8">
-        <v>9.2799999999999994</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -17459,7 +17503,7 @@
         <v>996</v>
       </c>
       <c r="D9">
-        <v>9.24</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -17467,7 +17511,7 @@
         <v>986</v>
       </c>
       <c r="D10">
-        <v>9.26</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -17475,7 +17519,7 @@
         <v>996</v>
       </c>
       <c r="D11">
-        <v>9.27</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -17483,7 +17527,7 @@
         <v>996</v>
       </c>
       <c r="D12">
-        <v>9.27</v>
+        <v>9.41</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -17491,7 +17535,7 @@
         <v>986</v>
       </c>
       <c r="D13">
-        <v>9.26</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -17499,7 +17543,7 @@
         <v>996</v>
       </c>
       <c r="D14">
-        <v>9.3000000000000007</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -17507,7 +17551,7 @@
         <v>996</v>
       </c>
       <c r="D15">
-        <v>9.1999999999999993</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -17515,7 +17559,7 @@
         <v>986</v>
       </c>
       <c r="D16">
-        <v>9.23</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -17523,7 +17567,7 @@
         <v>996</v>
       </c>
       <c r="D17">
-        <v>9.2100000000000009</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -17531,7 +17575,7 @@
         <v>996</v>
       </c>
       <c r="D18">
-        <v>9.26</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -17539,7 +17583,7 @@
         <v>986</v>
       </c>
       <c r="D19">
-        <v>9.26</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -17547,7 +17591,7 @@
         <v>996</v>
       </c>
       <c r="D20">
-        <v>9.2899999999999991</v>
+        <v>9.3699999999999992</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -17555,7 +17599,7 @@
         <v>996</v>
       </c>
       <c r="D21">
-        <v>9.26</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -17563,7 +17607,7 @@
         <v>986</v>
       </c>
       <c r="D22">
-        <v>9.19</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -17571,7 +17615,7 @@
         <v>996</v>
       </c>
       <c r="D23">
-        <v>9.2799999999999994</v>
+        <v>9.3800000000000008</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -17579,7 +17623,7 @@
         <v>996</v>
       </c>
       <c r="D24">
-        <v>9.27</v>
+        <v>9.4700000000000006</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -17587,7 +17631,7 @@
         <v>986</v>
       </c>
       <c r="D25">
-        <v>9.24</v>
+        <v>9.4700000000000006</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -17595,7 +17639,7 @@
         <v>996</v>
       </c>
       <c r="D26">
-        <v>9.23</v>
+        <v>9.3800000000000008</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -17603,7 +17647,7 @@
         <v>996</v>
       </c>
       <c r="D27">
-        <v>9.24</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -17611,7 +17655,7 @@
         <v>986</v>
       </c>
       <c r="D28">
-        <v>9.23</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -17619,7 +17663,7 @@
         <v>996</v>
       </c>
       <c r="D29">
-        <v>9.27</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -17627,7 +17671,7 @@
         <v>996</v>
       </c>
       <c r="D30">
-        <v>9.24</v>
+        <v>9.48</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -17635,7 +17679,7 @@
         <v>986</v>
       </c>
       <c r="D31">
-        <v>9.2799999999999994</v>
+        <v>9.39</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -17643,7 +17687,7 @@
         <v>996</v>
       </c>
       <c r="D32">
-        <v>9.2100000000000009</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -17651,7 +17695,7 @@
         <v>996</v>
       </c>
       <c r="D33">
-        <v>9.2799999999999994</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -17659,7 +17703,7 @@
         <v>986</v>
       </c>
       <c r="D34">
-        <v>9.25</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -17667,7 +17711,7 @@
         <v>996</v>
       </c>
       <c r="D35">
-        <v>9.27</v>
+        <v>9.31</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -17675,7 +17719,7 @@
         <v>996</v>
       </c>
       <c r="D36">
-        <v>9.26</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -17683,7 +17727,7 @@
         <v>986</v>
       </c>
       <c r="D37">
-        <v>9.24</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -17691,7 +17735,7 @@
         <v>996</v>
       </c>
       <c r="D38">
-        <v>9.25</v>
+        <v>9.52</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -17699,7 +17743,7 @@
         <v>996</v>
       </c>
       <c r="D39">
-        <v>9.2799999999999994</v>
+        <v>9.52</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -17707,7 +17751,7 @@
         <v>986</v>
       </c>
       <c r="D40">
-        <v>9.24</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -17715,7 +17759,7 @@
         <v>996</v>
       </c>
       <c r="D41">
-        <v>9.24</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -17723,7 +17767,7 @@
         <v>996</v>
       </c>
       <c r="D42">
-        <v>9.31</v>
+        <v>9.34</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -17731,7 +17775,7 @@
         <v>986</v>
       </c>
       <c r="D43">
-        <v>9.23</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -17739,7 +17783,7 @@
         <v>996</v>
       </c>
       <c r="D44">
-        <v>9.25</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -17747,7 +17791,7 @@
         <v>996</v>
       </c>
       <c r="D45">
-        <v>9.2200000000000006</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -17755,7 +17799,7 @@
         <v>986</v>
       </c>
       <c r="D46">
-        <v>9.2100000000000009</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -17771,7 +17815,7 @@
         <v>996</v>
       </c>
       <c r="D48">
-        <v>9.26</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -17779,7 +17823,7 @@
         <v>986</v>
       </c>
       <c r="D49">
-        <v>9.2799999999999994</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -17787,7 +17831,7 @@
         <v>996</v>
       </c>
       <c r="D50">
-        <v>9.24</v>
+        <v>9.52</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -17795,7 +17839,7 @@
         <v>996</v>
       </c>
       <c r="D51">
-        <v>9.2799999999999994</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -17803,7 +17847,7 @@
         <v>986</v>
       </c>
       <c r="D52">
-        <v>9.24</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -17811,7 +17855,7 @@
         <v>996</v>
       </c>
       <c r="D53">
-        <v>9.25</v>
+        <v>9.2899999999999991</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -17819,7 +17863,7 @@
         <v>996</v>
       </c>
       <c r="D54">
-        <v>9.26</v>
+        <v>9.36</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -17827,7 +17871,7 @@
         <v>986</v>
       </c>
       <c r="D55">
-        <v>9.26</v>
+        <v>9.31</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -17835,7 +17879,7 @@
         <v>996</v>
       </c>
       <c r="D56">
-        <v>9.27</v>
+        <v>9.35</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -17843,7 +17887,7 @@
         <v>996</v>
       </c>
       <c r="D57">
-        <v>9.26</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -17851,7 +17895,7 @@
         <v>986</v>
       </c>
       <c r="D58">
-        <v>9.2799999999999994</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -17859,7 +17903,7 @@
         <v>996</v>
       </c>
       <c r="D59">
-        <v>9.24</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -17867,7 +17911,7 @@
         <v>996</v>
       </c>
       <c r="D60">
-        <v>9.24</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -17875,7 +17919,12 @@
         <v>986</v>
       </c>
       <c r="D61">
-        <v>9.2799999999999994</v>
+        <v>9.5500000000000007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="D62">
+        <v>9.5500000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>